<commit_message>
Finished export button for phantom tab.
- Using ActiveX method of writing to Excel file from MATLAB
- Adds new row to excel log file
- Date in first column, find matching column for fields in GUI table and
  sets the value in Excel file
- If file is already open in Excel, Workbook.ReadOnly will be 1 and MATLAB
  will display error message
- 'Export successful' message shows if data is successfully written to
  excel file

- Added code to create header row if excel file has no data
- Added code to create chart if not created yet. Chart SourceData and
  position will update in every Export callback
- Added code to create new column if new field is added. New column shows
  on chart as separate series
</commit_message>
<xml_diff>
--- a/Log/ProstateBrachyQA Log.xlsx
+++ b/Log/ProstateBrachyQA Log.xlsx
@@ -16,9 +16,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>Weight</t>
+  </si>
+  <si>
+    <t>Test</t>
   </si>
 </sst>
 </file>
@@ -62,9 +65,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -78,6 +83,229 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-CA"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Phantom!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Weight</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Phantom!$A$2:$A$7</c:f>
+              <c:numCache>
+                <c:formatCode>d\-mmm\-yy</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>42205</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>42206</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>42207</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Phantom!$B$2:$B$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1100</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1200</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Phantom!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Test</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Phantom!$A$2:$A$7</c:f>
+              <c:numCache>
+                <c:formatCode>d\-mmm\-yy</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>42205</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>42206</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>42207</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Phantom!$C$2:$C$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="2">
+                  <c:v>10</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="64717952"/>
+        <c:axId val="64237568"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="64717952"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="d\-mmm\-yy" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr rot="-2100000" vert="horz"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="64237568"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="64237568"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="64717952"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>127000</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>431800</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -367,10 +595,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="A1:B2"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -379,19 +607,54 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="3"/>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1"/>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
+        <v>42205</v>
+      </c>
+      <c r="B2" s="3">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
         <v>42206</v>
       </c>
+      <c r="B3" s="3">
+        <v>1100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="4">
+        <v>42207</v>
+      </c>
+      <c r="B4">
+        <v>1200</v>
+      </c>
+      <c r="C4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="4"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="4"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Use number of rows/cols for chart data range instead of Sheet.UsedRange.
- If column was deleted from excel file, using UsedRange would still plot
  series for empty cells
- Update numRows and numCols variables directly when adding new row or new
  column.
</commit_message>
<xml_diff>
--- a/Log/ProstateBrachyQA Log.xlsx
+++ b/Log/ProstateBrachyQA Log.xlsx
@@ -16,12 +16,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
   <si>
     <t>Weight</t>
-  </si>
-  <si>
-    <t>Test</t>
   </si>
 </sst>
 </file>
@@ -99,6 +96,10 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
@@ -121,10 +122,10 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>Phantom!$A$2:$A$7</c:f>
+              <c:f>Phantom!$A$2:$A$4</c:f>
               <c:numCache>
                 <c:formatCode>d\-mmm\-yy</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>42205</c:v>
                 </c:pt>
@@ -139,10 +140,10 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Phantom!$B$2:$B$7</c:f>
+              <c:f>Phantom!$B$2:$B$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>1000</c:v>
                 </c:pt>
@@ -150,53 +151,7 @@
                   <c:v>1100</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1200</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Phantom!$C$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Test</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:xVal>
-            <c:numRef>
-              <c:f>Phantom!$A$2:$A$7</c:f>
-              <c:numCache>
-                <c:formatCode>d\-mmm\-yy</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>42205</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>42206</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>42207</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Phantom!$C$2:$C$7</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="2">
-                  <c:v>10</c:v>
+                  <c:v>1300</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -211,11 +166,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="64717952"/>
-        <c:axId val="64237568"/>
+        <c:axId val="55049216"/>
+        <c:axId val="53861760"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="64717952"/>
+        <c:axId val="55049216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -235,12 +190,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="64237568"/>
+        <c:crossAx val="53861760"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="64237568"/>
+        <c:axId val="53861760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -251,7 +206,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="64717952"/>
+        <c:crossAx val="55049216"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -598,7 +553,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="A5" sqref="A4:B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -611,9 +566,7 @@
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
+      <c r="C1" s="1"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
@@ -636,10 +589,7 @@
         <v>42207</v>
       </c>
       <c r="B4">
-        <v>1200</v>
-      </c>
-      <c r="C4">
-        <v>10</v>
+        <v>1300</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Freeze top row and make top row bold for phantom export.
</commit_message>
<xml_diff>
--- a/Log/ProstateBrachyQA Log.xlsx
+++ b/Log/ProstateBrachyQA Log.xlsx
@@ -8,7 +8,7 @@
   </bookViews>
   <sheets>
     <sheet name="Phantom" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Grayscale" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
@@ -122,36 +122,30 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>Phantom!$A$2:$A$4</c:f>
+              <c:f>Phantom!$A$2:$A$3</c:f>
               <c:numCache>
                 <c:formatCode>d\-mmm\-yy</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>42205</c:v>
+                  <c:v>42206</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>42206</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>42207</c:v>
+                  <c:v>42208</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Phantom!$B$2:$B$4</c:f>
+              <c:f>Phantom!$B$2:$B$3</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="2"/>
                 <c:pt idx="0">
                   <c:v>1000</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>1100</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1300</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -166,11 +160,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="55049216"/>
-        <c:axId val="53861760"/>
+        <c:axId val="50502656"/>
+        <c:axId val="50508544"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="55049216"/>
+        <c:axId val="50502656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -190,12 +184,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="53861760"/>
+        <c:crossAx val="50508544"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="53861760"/>
+        <c:axId val="50508544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -206,7 +200,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="55049216"/>
+        <c:crossAx val="50502656"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -234,13 +228,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>127000</xdr:colOff>
-      <xdr:row>5</xdr:row>
+      <xdr:row>4</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>431800</xdr:colOff>
-      <xdr:row>19</xdr:row>
+      <xdr:row>18</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -550,10 +544,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A4:B5"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3:B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -561,44 +556,37 @@
     <col min="1" max="1" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="3"/>
+    <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
-        <v>42205</v>
+        <v>42206</v>
       </c>
       <c r="B2" s="3">
         <v>1000</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
-        <v>42206</v>
+        <v>42208</v>
       </c>
       <c r="B3" s="3">
         <v>1100</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="4">
-        <v>42207</v>
-      </c>
-      <c r="B4">
-        <v>1300</v>
-      </c>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="4"/>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Improved segmentation code to work with new images.
- Use decreasing window size for adaptivethreshold from 150 to 70 if
  circle/ellipse is not found.
- Added check that major and minor axis lengths are similar for
  segmentCircle and segmentCrossSection
- Added check that segmented shape is in reasonable position (shape near
  edges of image is considered a false detection, continue searching)
</commit_message>
<xml_diff>
--- a/Log/ProstateBrachyQA Log.xlsx
+++ b/Log/ProstateBrachyQA Log.xlsx
@@ -16,9 +16,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>Weight</t>
+  </si>
+  <si>
+    <t>TEst</t>
   </si>
 </sst>
 </file>
@@ -64,10 +67,10 @@
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -96,10 +99,6 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:layout/>
-      <c:overlay val="0"/>
-    </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
@@ -122,14 +121,17 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>Phantom!$A$2:$A$3</c:f>
+              <c:f>Phantom!$A$2:$A$4</c:f>
               <c:numCache>
                 <c:formatCode>d\-mmm\-yy</c:formatCode>
-                <c:ptCount val="2"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>42206</c:v>
+                  <c:v>42207</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>42208</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>42208</c:v>
                 </c:pt>
               </c:numCache>
@@ -137,15 +139,64 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Phantom!$B$2:$B$3</c:f>
+              <c:f>Phantom!$B$2:$B$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="2"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>1000</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>1100</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1100</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Phantom!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>TEst</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Phantom!$A$2:$A$4</c:f>
+              <c:numCache>
+                <c:formatCode>d\-mmm\-yy</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>42207</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>42208</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>42208</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Phantom!$C$2:$C$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="2">
+                  <c:v>120</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -160,11 +211,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="50502656"/>
-        <c:axId val="50508544"/>
+        <c:axId val="50633728"/>
+        <c:axId val="50639616"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="50502656"/>
+        <c:axId val="50633728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -184,12 +235,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="50508544"/>
+        <c:crossAx val="50639616"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="50508544"/>
+        <c:axId val="50639616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -200,7 +251,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="50502656"/>
+        <c:crossAx val="50633728"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -228,13 +279,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>127000</xdr:colOff>
-      <xdr:row>4</xdr:row>
+      <xdr:row>5</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>431800</xdr:colOff>
-      <xdr:row>18</xdr:row>
+      <xdr:row>19</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -544,11 +595,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3:B3"/>
+      <selection pane="bottomLeft" activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -556,38 +607,49 @@
     <col min="1" max="1" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="1" t="s">
+    <row r="1" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="4" t="s">
         <v>0</v>
       </c>
+      <c r="C1" s="4" t="s">
+        <v>1</v>
+      </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="2">
-        <v>42206</v>
-      </c>
-      <c r="B2" s="3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>42207</v>
+      </c>
+      <c r="B2" s="2">
         <v>1000</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
         <v>42208</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B3" s="2">
         <v>1100</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="4"/>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="3">
+        <v>42208</v>
+      </c>
+      <c r="B4">
+        <v>1100</v>
+      </c>
+      <c r="C4">
+        <v>120</v>
+      </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="4"/>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="3"/>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="4"/>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="3"/>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="4"/>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added grayscale test export button.
</commit_message>
<xml_diff>
--- a/Log/ProstateBrachyQA Log.xlsx
+++ b/Log/ProstateBrachyQA Log.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="45" windowWidth="18195" windowHeight="12075"/>
+    <workbookView xWindow="480" yWindow="45" windowWidth="18195" windowHeight="12075" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Phantom" sheetId="1" r:id="rId1"/>
@@ -16,12 +16,24 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="6">
   <si>
     <t>Weight</t>
   </si>
   <si>
-    <t>TEst</t>
+    <t>Gradient Length</t>
+  </si>
+  <si>
+    <t>Baseline (mm)</t>
+  </si>
+  <si>
+    <t>Current (mm)</t>
+  </si>
+  <si>
+    <t>Result</t>
+  </si>
+  <si>
+    <t>PASS</t>
   </si>
 </sst>
 </file>
@@ -99,6 +111,9 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+    </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
@@ -121,82 +136,30 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>Phantom!$A$2:$A$4</c:f>
+              <c:f>Phantom!$A$2:$A$3</c:f>
               <c:numCache>
                 <c:formatCode>d\-mmm\-yy</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="2"/>
                 <c:pt idx="0">
                   <c:v>42207</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>42208</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>42208</c:v>
+                  <c:v>42214</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Phantom!$B$2:$B$4</c:f>
+              <c:f>Phantom!$B$2:$B$3</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="2"/>
                 <c:pt idx="0">
                   <c:v>1000</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1100</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1100</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Phantom!$C$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>TEst</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:xVal>
-            <c:numRef>
-              <c:f>Phantom!$A$2:$A$4</c:f>
-              <c:numCache>
-                <c:formatCode>d\-mmm\-yy</c:formatCode>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>42207</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>42208</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>42208</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Phantom!$C$2:$C$4</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
-                <c:pt idx="2">
-                  <c:v>120</c:v>
+                  <c:v>1500</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -211,11 +174,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="50633728"/>
-        <c:axId val="50639616"/>
+        <c:axId val="61381632"/>
+        <c:axId val="61387520"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="50633728"/>
+        <c:axId val="61381632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -235,12 +198,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="50639616"/>
+        <c:crossAx val="61387520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="50639616"/>
+        <c:axId val="61387520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -251,7 +214,207 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="50633728"/>
+        <c:crossAx val="61381632"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-CA"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Gradient Length</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Grayscale!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Baseline (mm)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Grayscale!$A$2:$A$3</c:f>
+              <c:numCache>
+                <c:formatCode>d\-mmm\-yy</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>42213</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>42214</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Grayscale!$B$2:$B$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>10.7</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10.7</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Grayscale!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Current (mm)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Grayscale!$A$2:$A$3</c:f>
+              <c:numCache>
+                <c:formatCode>d\-mmm\-yy</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>42213</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>42214</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Grayscale!$C$2:$C$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>11.06</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="64489344"/>
+        <c:axId val="64490880"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="64489344"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="d\-mmm\-yy" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr rot="-2100000" vert="horz"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="64490880"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="64490880"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="64489344"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -279,13 +442,48 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>127000</xdr:colOff>
-      <xdr:row>5</xdr:row>
+      <xdr:row>4</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>431800</xdr:colOff>
-      <xdr:row>19</xdr:row>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>127000</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>203200</xdr:colOff>
+      <xdr:row>18</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -595,11 +793,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3:B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -607,15 +805,12 @@
     <col min="1" max="1" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="4" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>42207</v>
       </c>
@@ -623,32 +818,24 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>42208</v>
+        <v>42214</v>
       </c>
       <c r="B3" s="2">
-        <v>1100</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="3">
-        <v>42208</v>
-      </c>
-      <c r="B4">
-        <v>1100</v>
-      </c>
-      <c r="C4">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="3"/>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="3"/>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>
     </row>
   </sheetData>
@@ -660,13 +847,76 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="D3" sqref="A3:D3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="3">
+        <v>42213</v>
+      </c>
+      <c r="B2">
+        <v>10.7</v>
+      </c>
+      <c r="C2">
+        <v>11</v>
+      </c>
+      <c r="D2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="3">
+        <v>42214</v>
+      </c>
+      <c r="B3">
+        <v>10.7</v>
+      </c>
+      <c r="C3">
+        <v>11.06</v>
+      </c>
+      <c r="D3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="3"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="3"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="3"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Export: put title in first cell and colour cell yellow.
</commit_message>
<xml_diff>
--- a/Log/ProstateBrachyQA Log.xlsx
+++ b/Log/ProstateBrachyQA Log.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="45" windowWidth="18195" windowHeight="12075" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="45" windowWidth="18195" windowHeight="12075"/>
   </bookViews>
   <sheets>
     <sheet name="Phantom" sheetId="1" r:id="rId1"/>
@@ -16,10 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="6">
-  <si>
-    <t>Weight</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Gradient Length</t>
   </si>
@@ -34,6 +31,12 @@
   </si>
   <si>
     <t>PASS</t>
+  </si>
+  <si>
+    <t>Phantom</t>
+  </si>
+  <si>
+    <t>Weight</t>
   </si>
 </sst>
 </file>
@@ -57,12 +60,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="13"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -77,12 +86,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -112,6 +122,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -141,10 +152,10 @@
                 <c:formatCode>d\-mmm\-yy</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>42207</c:v>
+                  <c:v>42214</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>42214</c:v>
+                  <c:v>42215</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -156,10 +167,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>1000</c:v>
+                  <c:v>1500</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1500</c:v>
+                  <c:v>1600</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -174,11 +185,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="61381632"/>
-        <c:axId val="61387520"/>
+        <c:axId val="65986560"/>
+        <c:axId val="65988096"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="61381632"/>
+        <c:axId val="65986560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -198,12 +209,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="61387520"/>
+        <c:crossAx val="65988096"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="61387520"/>
+        <c:axId val="65988096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -214,13 +225,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="61381632"/>
+        <c:crossAx val="65986560"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -265,7 +277,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -290,29 +301,23 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>Grayscale!$A$2:$A$3</c:f>
+              <c:f>Grayscale!$A$2</c:f>
               <c:numCache>
                 <c:formatCode>d\-mmm\-yy</c:formatCode>
-                <c:ptCount val="2"/>
+                <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>42213</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>42214</c:v>
+                  <c:v>42215</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Grayscale!$B$2:$B$3</c:f>
+              <c:f>Grayscale!$B$2</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="2"/>
+                <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>10.7</c:v>
-                </c:pt>
-                <c:pt idx="1">
                   <c:v>10.7</c:v>
                 </c:pt>
               </c:numCache>
@@ -336,29 +341,23 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>Grayscale!$A$2:$A$3</c:f>
+              <c:f>Grayscale!$A$2</c:f>
               <c:numCache>
                 <c:formatCode>d\-mmm\-yy</c:formatCode>
-                <c:ptCount val="2"/>
+                <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>42213</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>42214</c:v>
+                  <c:v>42215</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Grayscale!$C$2:$C$3</c:f>
+              <c:f>Grayscale!$C$2</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="2"/>
+                <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>11</c:v>
-                </c:pt>
-                <c:pt idx="1">
                   <c:v>11.06</c:v>
                 </c:pt>
               </c:numCache>
@@ -374,11 +373,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="64489344"/>
-        <c:axId val="64490880"/>
+        <c:axId val="66181760"/>
+        <c:axId val="67514752"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="64489344"/>
+        <c:axId val="66181760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -398,12 +397,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="64490880"/>
+        <c:crossAx val="67514752"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="64490880"/>
+        <c:axId val="67514752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -414,14 +413,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="64489344"/>
+        <c:crossAx val="66181760"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -447,7 +445,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>431800</xdr:colOff>
+      <xdr:colOff>546100</xdr:colOff>
       <xdr:row>18</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
@@ -477,13 +475,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>127000</xdr:colOff>
-      <xdr:row>4</xdr:row>
+      <xdr:row>3</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>203200</xdr:colOff>
-      <xdr:row>18</xdr:row>
+      <xdr:row>17</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -795,35 +793,39 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3:B4"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" customWidth="1"/>
+    <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>5</v>
+      </c>
       <c r="B1" s="4" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>42207</v>
+        <v>42214</v>
       </c>
       <c r="B2" s="2">
-        <v>1000</v>
+        <v>1500</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>42214</v>
+        <v>42215</v>
       </c>
       <c r="B3" s="2">
-        <v>1500</v>
+        <v>1600</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -847,11 +849,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="D3" sqref="A3:D3"/>
+      <selection pane="bottomLeft" activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -863,55 +865,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
-        <v>42213</v>
+        <v>42215</v>
       </c>
       <c r="B2">
         <v>10.7</v>
       </c>
       <c r="C2">
-        <v>11</v>
+        <v>11.06</v>
       </c>
       <c r="D2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="3">
-        <v>42214</v>
-      </c>
-      <c r="B3">
-        <v>10.7</v>
-      </c>
-      <c r="C3">
-        <v>11.06</v>
-      </c>
-      <c r="D3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="3"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="3"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="3"/>
+        <v>4</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added depth test export
- Longitudinal plane data is shown to the right of axial plane data
- 2 separate charts for axial and longitudinal
</commit_message>
<xml_diff>
--- a/Log/ProstateBrachyQA Log.xlsx
+++ b/Log/ProstateBrachyQA Log.xlsx
@@ -4,19 +4,25 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="45" windowWidth="18195" windowHeight="12075"/>
+    <workbookView xWindow="480" yWindow="45" windowWidth="18195" windowHeight="12075" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Phantom" sheetId="1" r:id="rId1"/>
     <sheet name="Grayscale" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Depth" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="10">
+  <si>
+    <t>Phantom</t>
+  </si>
+  <si>
+    <t>Weight</t>
+  </si>
   <si>
     <t>Gradient Length</t>
   </si>
@@ -33,10 +39,13 @@
     <t>PASS</t>
   </si>
   <si>
-    <t>Phantom</t>
+    <t>Axial Plane</t>
   </si>
   <si>
-    <t>Weight</t>
+    <t>Longitudinal Plane</t>
+  </si>
+  <si>
+    <t>FAIL</t>
   </si>
 </sst>
 </file>
@@ -86,13 +95,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -122,7 +132,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -185,11 +194,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="65986560"/>
-        <c:axId val="65988096"/>
+        <c:axId val="60136448"/>
+        <c:axId val="60142336"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="65986560"/>
+        <c:axId val="60136448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -209,12 +218,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="65988096"/>
+        <c:crossAx val="60142336"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="65988096"/>
+        <c:axId val="60142336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -225,14 +234,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="65986560"/>
+        <c:crossAx val="60136448"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -373,11 +381,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="66181760"/>
-        <c:axId val="67514752"/>
+        <c:axId val="61540224"/>
+        <c:axId val="61541760"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="66181760"/>
+        <c:axId val="61540224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -397,12 +405,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="67514752"/>
+        <c:crossAx val="61541760"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="67514752"/>
+        <c:axId val="61541760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -413,13 +421,391 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="66181760"/>
+        <c:crossAx val="61540224"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-CA"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Depth (Axial)</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Depth!$B$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Baseline (mm)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Depth!$A$3</c:f>
+              <c:numCache>
+                <c:formatCode>d\-mmm\-yy</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>42215</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Depth!$B$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>75.3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Depth!$C$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Current (mm)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Depth!$A$3</c:f>
+              <c:numCache>
+                <c:formatCode>d\-mmm\-yy</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>42215</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Depth!$C$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>85.42</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="76538624"/>
+        <c:axId val="65574016"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="76538624"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="d\-mmm\-yy" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr rot="-2100000" vert="horz"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="65574016"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="65574016"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="76538624"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-CA"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Depth (Longitudinal)</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Depth!$E$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Baseline (mm)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Depth!$A$3</c:f>
+              <c:numCache>
+                <c:formatCode>d\-mmm\-yy</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>42215</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Depth!$E$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>78.8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Depth!$F$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Current (mm)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Depth!$A$3</c:f>
+              <c:numCache>
+                <c:formatCode>d\-mmm\-yy</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>42215</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Depth!$F$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>79.2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="77043200"/>
+        <c:axId val="76495488"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="77043200"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="d\-mmm\-yy" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr rot="-2100000" vert="horz"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="76495488"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="76495488"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="77043200"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -496,6 +882,71 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>127000</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>488950</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>127000</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>603250</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -793,7 +1244,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
     </sheetView>
@@ -806,10 +1257,10 @@
   <sheetData>
     <row r="1" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -849,11 +1300,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="F8" sqref="F8"/>
+      <selection pane="bottomLeft" activeCell="G5" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -866,16 +1317,16 @@
   <sheetData>
     <row r="1" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -889,8 +1340,11 @@
         <v>11.06</v>
       </c>
       <c r="D2" t="s">
-        <v>4</v>
-      </c>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -901,12 +1355,98 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="H29" sqref="A1:XFD1048576"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+    </row>
+    <row r="2" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="3">
+        <v>42215</v>
+      </c>
+      <c r="B3">
+        <v>75.3</v>
+      </c>
+      <c r="C3">
+        <v>85.42</v>
+      </c>
+      <c r="D3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3">
+        <v>78.8</v>
+      </c>
+      <c r="F3">
+        <v>79.2</v>
+      </c>
+      <c r="G3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="3"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="3"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="3"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="E1:G1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added axial resolution export
- 2 separate charts for axial and longitudinal plane data
- Separate series for each point (B1,F1,B5,F5 for axial, Filament 1 and
  Filament 6 for longitudinal)
- Update chart series data every export
</commit_message>
<xml_diff>
--- a/Log/ProstateBrachyQA Log.xlsx
+++ b/Log/ProstateBrachyQA Log.xlsx
@@ -4,19 +4,20 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="45" windowWidth="18195" windowHeight="12075" activeTab="2"/>
+    <workbookView xWindow="480" yWindow="45" windowWidth="18195" windowHeight="12075"/>
   </bookViews>
   <sheets>
     <sheet name="Phantom" sheetId="1" r:id="rId1"/>
     <sheet name="Grayscale" sheetId="2" r:id="rId2"/>
     <sheet name="Depth" sheetId="3" r:id="rId3"/>
+    <sheet name="Axial Resolution" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="19">
   <si>
     <t>Phantom</t>
   </si>
@@ -46,6 +47,33 @@
   </si>
   <si>
     <t>FAIL</t>
+  </si>
+  <si>
+    <t>Axial Resolution</t>
+  </si>
+  <si>
+    <t>Diff (abs)</t>
+  </si>
+  <si>
+    <t>Diff (%)</t>
+  </si>
+  <si>
+    <t>Proximal (B1)</t>
+  </si>
+  <si>
+    <t>Proximal (F1)</t>
+  </si>
+  <si>
+    <t>Distal (B5)</t>
+  </si>
+  <si>
+    <t>Distal (F5)</t>
+  </si>
+  <si>
+    <t>Filament 1</t>
+  </si>
+  <si>
+    <t>Filament 6</t>
   </si>
 </sst>
 </file>
@@ -95,13 +123,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="15" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -132,6 +159,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -194,11 +222,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="60136448"/>
-        <c:axId val="60142336"/>
+        <c:axId val="69927296"/>
+        <c:axId val="69928832"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="60136448"/>
+        <c:axId val="69927296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -218,12 +246,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="60142336"/>
+        <c:crossAx val="69928832"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="60142336"/>
+        <c:axId val="69928832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -234,13 +262,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="60136448"/>
+        <c:crossAx val="69927296"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -285,6 +314,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -381,11 +411,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="61540224"/>
-        <c:axId val="61541760"/>
+        <c:axId val="69991424"/>
+        <c:axId val="70275840"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="61540224"/>
+        <c:axId val="69991424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -405,12 +435,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="61541760"/>
+        <c:crossAx val="70275840"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="61541760"/>
+        <c:axId val="70275840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -421,13 +451,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="61540224"/>
+        <c:crossAx val="69991424"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -497,11 +528,14 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>Depth!$A$3</c:f>
+              <c:f>Depth!$A$3:$A$4</c:f>
               <c:numCache>
                 <c:formatCode>d\-mmm\-yy</c:formatCode>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>42215</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>42215</c:v>
                 </c:pt>
               </c:numCache>
@@ -509,11 +543,14 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Depth!$B$3</c:f>
+              <c:f>Depth!$B$3:$B$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>75.3</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>75.3</c:v>
                 </c:pt>
               </c:numCache>
@@ -537,11 +574,14 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>Depth!$A$3</c:f>
+              <c:f>Depth!$A$3:$A$4</c:f>
               <c:numCache>
                 <c:formatCode>d\-mmm\-yy</c:formatCode>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>42215</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>42215</c:v>
                 </c:pt>
               </c:numCache>
@@ -549,11 +589,14 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Depth!$C$3</c:f>
+              <c:f>Depth!$C$3:$C$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>85.42</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>85.42</c:v>
                 </c:pt>
               </c:numCache>
@@ -569,11 +612,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="76538624"/>
-        <c:axId val="65574016"/>
+        <c:axId val="70317952"/>
+        <c:axId val="70319488"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="76538624"/>
+        <c:axId val="70317952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -593,12 +636,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="65574016"/>
+        <c:crossAx val="70319488"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="65574016"/>
+        <c:axId val="70319488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -609,7 +652,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="76538624"/>
+        <c:crossAx val="70317952"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -686,11 +729,14 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>Depth!$A$3</c:f>
+              <c:f>Depth!$A$3:$A$4</c:f>
               <c:numCache>
                 <c:formatCode>d\-mmm\-yy</c:formatCode>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>42215</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>42215</c:v>
                 </c:pt>
               </c:numCache>
@@ -698,11 +744,14 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Depth!$E$3</c:f>
+              <c:f>Depth!$E$3:$E$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>78.8</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>78.8</c:v>
                 </c:pt>
               </c:numCache>
@@ -726,11 +775,14 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>Depth!$A$3</c:f>
+              <c:f>Depth!$A$3:$A$4</c:f>
               <c:numCache>
                 <c:formatCode>d\-mmm\-yy</c:formatCode>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>42215</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>42215</c:v>
                 </c:pt>
               </c:numCache>
@@ -738,11 +790,14 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Depth!$F$3</c:f>
+              <c:f>Depth!$F$3:$F$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>79.2</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>79.2</c:v>
                 </c:pt>
               </c:numCache>
@@ -758,11 +813,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="77043200"/>
-        <c:axId val="76495488"/>
+        <c:axId val="70418816"/>
+        <c:axId val="70420352"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="77043200"/>
+        <c:axId val="70418816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -782,12 +837,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="76495488"/>
+        <c:crossAx val="70420352"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="76495488"/>
+        <c:axId val="70420352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -798,7 +853,453 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="77043200"/>
+        <c:crossAx val="70418816"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-CA"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Axial Resolution (Axial)</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Proximal (B1)</c:v>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>('Axial Resolution'!$A$3,'Axial Resolution'!$A$8)</c:f>
+              <c:numCache>
+                <c:formatCode>d\-mmm\-yy</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>42214</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>42215</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>('Axial Resolution'!$D$3,'Axial Resolution'!$D$8)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>0.77</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.46</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Proximal (F1)</c:v>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>('Axial Resolution'!$A$3,'Axial Resolution'!$A$8)</c:f>
+              <c:numCache>
+                <c:formatCode>d\-mmm\-yy</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>42214</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>42215</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>('Axial Resolution'!$D$4,'Axial Resolution'!$D$9)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>0.51</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.53</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>Distal (B5)</c:v>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>('Axial Resolution'!$A$3,'Axial Resolution'!$A$8)</c:f>
+              <c:numCache>
+                <c:formatCode>d\-mmm\-yy</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>42214</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>42215</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>('Axial Resolution'!$D$5,'Axial Resolution'!$D$10)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>0.73</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.57999999999999996</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>Distal (F5)</c:v>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>('Axial Resolution'!$A$3,'Axial Resolution'!$A$8)</c:f>
+              <c:numCache>
+                <c:formatCode>d\-mmm\-yy</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>42214</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>42215</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>('Axial Resolution'!$D$6,'Axial Resolution'!$D$11)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>0.69</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.62</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="70494464"/>
+        <c:axId val="70508544"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="70494464"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="d\-mmm\-yy" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr rot="-2100000" vert="horz"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="70508544"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="70508544"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="70494464"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-CA"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Axial Resolution (Longitudinal)</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Filament 1</c:v>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>('Axial Resolution'!$A$3,'Axial Resolution'!$A$8)</c:f>
+              <c:numCache>
+                <c:formatCode>d\-mmm\-yy</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>42214</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>42215</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>('Axial Resolution'!$J$3,'Axial Resolution'!$J$8)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>0.61</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Filament 6</c:v>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>('Axial Resolution'!$A$3,'Axial Resolution'!$A$8)</c:f>
+              <c:numCache>
+                <c:formatCode>d\-mmm\-yy</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>42214</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>42215</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>('Axial Resolution'!$J$4,'Axial Resolution'!$J$9)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>0.47</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.48</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="70787840"/>
+        <c:axId val="70789376"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="70787840"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="d\-mmm\-yy" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr rot="-2100000" vert="horz"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="70789376"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="70789376"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="70787840"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -896,13 +1397,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>127000</xdr:colOff>
-      <xdr:row>4</xdr:row>
+      <xdr:row>5</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>488950</xdr:colOff>
-      <xdr:row>18</xdr:row>
+      <xdr:row>19</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -926,13 +1427,78 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>127000</xdr:colOff>
-      <xdr:row>4</xdr:row>
+      <xdr:row>5</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
       <xdr:colOff>603250</xdr:colOff>
-      <xdr:row>18</xdr:row>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>127000</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>384175</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>127000</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>203200</xdr:colOff>
+      <xdr:row>26</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1244,52 +1810,52 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomLeft" sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
+      <c r="A2" s="4">
         <v>42214</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2" s="1">
         <v>1500</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
+      <c r="A3" s="4">
         <v>42215</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B3" s="1">
         <v>1600</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="3"/>
+      <c r="A4" s="4"/>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="3"/>
+      <c r="A5" s="4"/>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="3"/>
+      <c r="A6" s="4"/>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="3"/>
+      <c r="A7" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1304,33 +1870,33 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="G5" sqref="A1:XFD1048576"/>
+      <selection pane="bottomLeft" sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.42578125" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="3">
+      <c r="A2" s="4">
         <v>42215</v>
       </c>
       <c r="B2">
@@ -1344,7 +1910,7 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="3"/>
+      <c r="A3" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1357,14 +1923,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="H29" sqref="A1:XFD1048576"/>
+      <selection pane="bottomLeft" activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.42578125" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6.5703125" bestFit="1" customWidth="1"/>
@@ -1373,43 +1939,43 @@
     <col min="7" max="7" width="6.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6" t="s">
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-    </row>
-    <row r="2" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="4" t="s">
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+    </row>
+    <row r="2" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="G2" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="3">
+      <c r="A3" s="4">
         <v>42215</v>
       </c>
       <c r="B3">
@@ -1432,13 +1998,33 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="3"/>
+      <c r="A4" s="4">
+        <v>42215</v>
+      </c>
+      <c r="B4">
+        <v>75.3</v>
+      </c>
+      <c r="C4">
+        <v>85.42</v>
+      </c>
+      <c r="D4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4">
+        <v>78.8</v>
+      </c>
+      <c r="F4">
+        <v>79.2</v>
+      </c>
+      <c r="G4" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="3"/>
+      <c r="A5" s="4"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="3"/>
+      <c r="A6" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1449,4 +2035,350 @@
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="6.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
+      <c r="K1" s="5"/>
+      <c r="L1" s="5"/>
+    </row>
+    <row r="2" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" s="4">
+        <v>42214</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3">
+        <v>0.41</v>
+      </c>
+      <c r="D3">
+        <v>0.77</v>
+      </c>
+      <c r="E3">
+        <v>0.36</v>
+      </c>
+      <c r="F3">
+        <v>60.99</v>
+      </c>
+      <c r="G3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I3">
+        <v>0.44</v>
+      </c>
+      <c r="J3">
+        <v>0.61</v>
+      </c>
+      <c r="K3">
+        <v>0.17</v>
+      </c>
+      <c r="L3">
+        <v>32.72</v>
+      </c>
+      <c r="M3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="D4">
+        <v>0.51</v>
+      </c>
+      <c r="E4">
+        <v>0.04</v>
+      </c>
+      <c r="F4">
+        <v>6.79</v>
+      </c>
+      <c r="G4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I4">
+        <v>0.44</v>
+      </c>
+      <c r="J4">
+        <v>0.47</v>
+      </c>
+      <c r="K4">
+        <v>0.03</v>
+      </c>
+      <c r="L4">
+        <v>6.65</v>
+      </c>
+      <c r="M4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5">
+        <v>0.69</v>
+      </c>
+      <c r="D5">
+        <v>0.73</v>
+      </c>
+      <c r="E5">
+        <v>0.04</v>
+      </c>
+      <c r="F5">
+        <v>5.86</v>
+      </c>
+      <c r="G5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B6" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6">
+        <v>0.5</v>
+      </c>
+      <c r="D6">
+        <v>0.69</v>
+      </c>
+      <c r="E6">
+        <v>0.19</v>
+      </c>
+      <c r="F6">
+        <v>31.48</v>
+      </c>
+      <c r="G6" t="s">
+        <v>6</v>
+      </c>
+      <c r="H6" s="2"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" s="4"/>
+      <c r="B7" s="2"/>
+      <c r="H7" s="2"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" s="4">
+        <v>42215</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8">
+        <v>0.41</v>
+      </c>
+      <c r="D8">
+        <v>0.46</v>
+      </c>
+      <c r="E8">
+        <v>0.05</v>
+      </c>
+      <c r="F8">
+        <v>11.97</v>
+      </c>
+      <c r="G8" t="s">
+        <v>6</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I8">
+        <v>0.44</v>
+      </c>
+      <c r="J8">
+        <v>0.5</v>
+      </c>
+      <c r="K8">
+        <v>0.06</v>
+      </c>
+      <c r="L8">
+        <v>13.36</v>
+      </c>
+      <c r="M8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B9" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="D9">
+        <v>0.53</v>
+      </c>
+      <c r="E9">
+        <v>0.02</v>
+      </c>
+      <c r="F9">
+        <v>3.65</v>
+      </c>
+      <c r="G9" t="s">
+        <v>6</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I9">
+        <v>0.44</v>
+      </c>
+      <c r="J9">
+        <v>0.48</v>
+      </c>
+      <c r="K9">
+        <v>0.04</v>
+      </c>
+      <c r="L9">
+        <v>9.67</v>
+      </c>
+      <c r="M9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B10" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10">
+        <v>0.69</v>
+      </c>
+      <c r="D10">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="E10">
+        <v>0.11</v>
+      </c>
+      <c r="F10">
+        <v>17.239999999999998</v>
+      </c>
+      <c r="G10" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B11" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11">
+        <v>0.5</v>
+      </c>
+      <c r="D11">
+        <v>0.62</v>
+      </c>
+      <c r="E11">
+        <v>0.12</v>
+      </c>
+      <c r="F11">
+        <v>21.39</v>
+      </c>
+      <c r="G11" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13" s="4"/>
+      <c r="B13" s="2"/>
+      <c r="H13" s="2"/>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B14" s="2"/>
+      <c r="H14" s="2"/>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B15" s="2"/>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B16" s="2"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B1:G1"/>
+    <mergeCell ref="H1:L1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added lateral resolution export.
</commit_message>
<xml_diff>
--- a/Log/ProstateBrachyQA Log.xlsx
+++ b/Log/ProstateBrachyQA Log.xlsx
@@ -4,20 +4,21 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="45" windowWidth="18195" windowHeight="12075"/>
+    <workbookView xWindow="480" yWindow="45" windowWidth="18195" windowHeight="12075" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Phantom" sheetId="1" r:id="rId1"/>
     <sheet name="Grayscale" sheetId="2" r:id="rId2"/>
     <sheet name="Depth" sheetId="3" r:id="rId3"/>
     <sheet name="Axial Resolution" sheetId="4" r:id="rId4"/>
+    <sheet name="Lateral Resolution" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="20">
   <si>
     <t>Phantom</t>
   </si>
@@ -74,6 +75,9 @@
   </si>
   <si>
     <t>Filament 6</t>
+  </si>
+  <si>
+    <t>Lateral Resolution</t>
   </si>
 </sst>
 </file>
@@ -159,7 +163,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -222,11 +225,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="69927296"/>
-        <c:axId val="69928832"/>
+        <c:axId val="62316544"/>
+        <c:axId val="62318080"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="69927296"/>
+        <c:axId val="62316544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -246,12 +249,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="69928832"/>
+        <c:crossAx val="62318080"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="69928832"/>
+        <c:axId val="62318080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -262,14 +265,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="69927296"/>
+        <c:crossAx val="62316544"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -314,7 +316,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -411,11 +412,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="69991424"/>
-        <c:axId val="70275840"/>
+        <c:axId val="63036032"/>
+        <c:axId val="63201664"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="69991424"/>
+        <c:axId val="63036032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -435,12 +436,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="70275840"/>
+        <c:crossAx val="63201664"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="70275840"/>
+        <c:axId val="63201664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -451,14 +452,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="69991424"/>
+        <c:crossAx val="63036032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -503,7 +503,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -612,11 +611,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="70317952"/>
-        <c:axId val="70319488"/>
+        <c:axId val="63215104"/>
+        <c:axId val="63216640"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="70317952"/>
+        <c:axId val="63215104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -636,12 +635,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="70319488"/>
+        <c:crossAx val="63216640"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="70319488"/>
+        <c:axId val="63216640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -652,14 +651,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="70317952"/>
+        <c:crossAx val="63215104"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -704,7 +702,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -813,11 +810,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="70418816"/>
-        <c:axId val="70420352"/>
+        <c:axId val="64307200"/>
+        <c:axId val="64308736"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="70418816"/>
+        <c:axId val="64307200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -837,12 +834,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="70420352"/>
+        <c:crossAx val="64308736"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="70420352"/>
+        <c:axId val="64308736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -853,14 +850,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="70418816"/>
+        <c:crossAx val="64307200"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -905,7 +901,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1074,11 +1069,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="70494464"/>
-        <c:axId val="70508544"/>
+        <c:axId val="64545152"/>
+        <c:axId val="64546688"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="70494464"/>
+        <c:axId val="64545152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1098,12 +1093,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="70508544"/>
+        <c:crossAx val="64546688"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="70508544"/>
+        <c:axId val="64546688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1114,14 +1109,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="70494464"/>
+        <c:crossAx val="64545152"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1166,7 +1160,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1259,11 +1252,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="70787840"/>
-        <c:axId val="70789376"/>
+        <c:axId val="52015104"/>
+        <c:axId val="52016640"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="70787840"/>
+        <c:axId val="52015104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1283,12 +1276,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="70789376"/>
+        <c:crossAx val="52016640"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="70789376"/>
+        <c:axId val="52016640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1299,7 +1292,452 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="70787840"/>
+        <c:crossAx val="52015104"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-CA"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Lateral Resolution (Axial)</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Proximal (B1)</c:v>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>('Lateral Resolution'!$A$3,'Lateral Resolution'!$A$8)</c:f>
+              <c:numCache>
+                <c:formatCode>d\-mmm\-yy</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>42214</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>42215</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>('Lateral Resolution'!$D$3,'Lateral Resolution'!$D$8)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>2.46</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.61</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Proximal (F1)</c:v>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>('Lateral Resolution'!$A$3,'Lateral Resolution'!$A$8)</c:f>
+              <c:numCache>
+                <c:formatCode>d\-mmm\-yy</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>42214</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>42215</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>('Lateral Resolution'!$D$4,'Lateral Resolution'!$D$9)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>2.7</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.23</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>Distal (B5)</c:v>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>('Lateral Resolution'!$A$3,'Lateral Resolution'!$A$8)</c:f>
+              <c:numCache>
+                <c:formatCode>d\-mmm\-yy</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>42214</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>42215</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>('Lateral Resolution'!$D$5,'Lateral Resolution'!$D$10)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>5.84</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.42</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>Distal (F5)</c:v>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>('Lateral Resolution'!$A$3,'Lateral Resolution'!$A$8)</c:f>
+              <c:numCache>
+                <c:formatCode>d\-mmm\-yy</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>42214</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>42215</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>('Lateral Resolution'!$D$6,'Lateral Resolution'!$D$11)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>6.24</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.47</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="64491904"/>
+        <c:axId val="64493440"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="64491904"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="d\-mmm\-yy" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr rot="-2100000" vert="horz"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="64493440"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="64493440"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="64491904"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-CA"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Lateral Resolution (Longitudinal)</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Filament 1</c:v>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>('Lateral Resolution'!$A$3,'Lateral Resolution'!$A$8)</c:f>
+              <c:numCache>
+                <c:formatCode>d\-mmm\-yy</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>42214</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>42215</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>('Lateral Resolution'!$J$3,'Lateral Resolution'!$J$8)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.74</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Filament 6</c:v>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>('Lateral Resolution'!$A$3,'Lateral Resolution'!$A$8)</c:f>
+              <c:numCache>
+                <c:formatCode>d\-mmm\-yy</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>42214</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>42215</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>('Lateral Resolution'!$J$4,'Lateral Resolution'!$J$9)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>1.76</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="64584320"/>
+        <c:axId val="64586112"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="64584320"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="d\-mmm\-yy" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr rot="-2100000" vert="horz"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="64586112"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="64586112"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="64584320"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1468,6 +1906,71 @@
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>384175</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>127000</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>203200</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>127000</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>269875</xdr:colOff>
       <xdr:row>26</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
@@ -1810,7 +2313,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
       <selection pane="bottomLeft" sqref="A1:A1048576"/>
     </sheetView>
@@ -2381,4 +2884,329 @@
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="6.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
+      <c r="K1" s="5"/>
+      <c r="L1" s="5"/>
+    </row>
+    <row r="2" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" s="4">
+        <v>42214</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3">
+        <v>1.27</v>
+      </c>
+      <c r="D3">
+        <v>2.46</v>
+      </c>
+      <c r="E3">
+        <v>1.19</v>
+      </c>
+      <c r="F3">
+        <v>63.64</v>
+      </c>
+      <c r="G3" t="s">
+        <v>9</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I3">
+        <v>1.1100000000000001</v>
+      </c>
+      <c r="J3">
+        <v>2</v>
+      </c>
+      <c r="K3">
+        <v>0.89</v>
+      </c>
+      <c r="L3">
+        <v>57.09</v>
+      </c>
+      <c r="M3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4">
+        <v>1.37</v>
+      </c>
+      <c r="D4">
+        <v>2.7</v>
+      </c>
+      <c r="E4">
+        <v>1.33</v>
+      </c>
+      <c r="F4">
+        <v>65.400000000000006</v>
+      </c>
+      <c r="G4" t="s">
+        <v>9</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I4">
+        <v>1</v>
+      </c>
+      <c r="J4">
+        <v>1.76</v>
+      </c>
+      <c r="K4">
+        <v>0.76</v>
+      </c>
+      <c r="L4">
+        <v>54.96</v>
+      </c>
+      <c r="M4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5">
+        <v>3.43</v>
+      </c>
+      <c r="D5">
+        <v>5.84</v>
+      </c>
+      <c r="E5">
+        <v>2.41</v>
+      </c>
+      <c r="F5">
+        <v>52.04</v>
+      </c>
+      <c r="G5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B6" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6">
+        <v>4.3</v>
+      </c>
+      <c r="D6">
+        <v>6.24</v>
+      </c>
+      <c r="E6">
+        <v>1.94</v>
+      </c>
+      <c r="F6">
+        <v>36.78</v>
+      </c>
+      <c r="G6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" s="4">
+        <v>42215</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8">
+        <v>1.27</v>
+      </c>
+      <c r="D8">
+        <v>2.61</v>
+      </c>
+      <c r="E8">
+        <v>1.34</v>
+      </c>
+      <c r="F8">
+        <v>69.03</v>
+      </c>
+      <c r="G8" t="s">
+        <v>9</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I8">
+        <v>1.1100000000000001</v>
+      </c>
+      <c r="J8">
+        <v>2.74</v>
+      </c>
+      <c r="K8">
+        <v>1.63</v>
+      </c>
+      <c r="L8">
+        <v>84.54</v>
+      </c>
+      <c r="M8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B9" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9">
+        <v>1.37</v>
+      </c>
+      <c r="D9">
+        <v>3.23</v>
+      </c>
+      <c r="E9">
+        <v>1.86</v>
+      </c>
+      <c r="F9">
+        <v>80.97</v>
+      </c>
+      <c r="G9" t="s">
+        <v>9</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I9">
+        <v>1</v>
+      </c>
+      <c r="J9">
+        <v>2.5</v>
+      </c>
+      <c r="K9">
+        <v>1.5</v>
+      </c>
+      <c r="L9">
+        <v>85.85</v>
+      </c>
+      <c r="M9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B10" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10">
+        <v>3.43</v>
+      </c>
+      <c r="D10">
+        <v>5.42</v>
+      </c>
+      <c r="E10">
+        <v>1.99</v>
+      </c>
+      <c r="F10">
+        <v>45.03</v>
+      </c>
+      <c r="G10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B11" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11">
+        <v>4.3</v>
+      </c>
+      <c r="D11">
+        <v>5.47</v>
+      </c>
+      <c r="E11">
+        <v>1.17</v>
+      </c>
+      <c r="F11">
+        <v>23.91</v>
+      </c>
+      <c r="G11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B1:G1"/>
+    <mergeCell ref="H1:L1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added axial distance export.
</commit_message>
<xml_diff>
--- a/Log/ProstateBrachyQA Log.xlsx
+++ b/Log/ProstateBrachyQA Log.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="45" windowWidth="18195" windowHeight="12075" activeTab="4"/>
+    <workbookView xWindow="480" yWindow="45" windowWidth="18195" windowHeight="12075" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Phantom" sheetId="1" r:id="rId1"/>
@@ -12,13 +12,14 @@
     <sheet name="Depth" sheetId="3" r:id="rId3"/>
     <sheet name="Axial Resolution" sheetId="4" r:id="rId4"/>
     <sheet name="Lateral Resolution" sheetId="5" r:id="rId5"/>
+    <sheet name="Axial Distance" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="25">
   <si>
     <t>Phantom</t>
   </si>
@@ -78,6 +79,21 @@
   </si>
   <si>
     <t>Lateral Resolution</t>
+  </si>
+  <si>
+    <t>Axial Distance</t>
+  </si>
+  <si>
+    <t>Known (mm)</t>
+  </si>
+  <si>
+    <t>Measured (mm)</t>
+  </si>
+  <si>
+    <t>B1 - B5</t>
+  </si>
+  <si>
+    <t>F1 - F5</t>
   </si>
 </sst>
 </file>
@@ -225,11 +241,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="62316544"/>
-        <c:axId val="62318080"/>
+        <c:axId val="63635840"/>
+        <c:axId val="63637376"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="62316544"/>
+        <c:axId val="63635840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -249,12 +265,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="62318080"/>
+        <c:crossAx val="63637376"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="62318080"/>
+        <c:axId val="63637376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -265,7 +281,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="62316544"/>
+        <c:crossAx val="63635840"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -412,11 +428,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="63036032"/>
-        <c:axId val="63201664"/>
+        <c:axId val="63699968"/>
+        <c:axId val="64254720"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="63036032"/>
+        <c:axId val="63699968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -436,12 +452,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="63201664"/>
+        <c:crossAx val="64254720"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="63201664"/>
+        <c:axId val="64254720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -452,7 +468,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="63036032"/>
+        <c:crossAx val="63699968"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -611,11 +627,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="63215104"/>
-        <c:axId val="63216640"/>
+        <c:axId val="64276352"/>
+        <c:axId val="64277888"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="63215104"/>
+        <c:axId val="64276352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -635,12 +651,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="63216640"/>
+        <c:crossAx val="64277888"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="63216640"/>
+        <c:axId val="64277888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -651,7 +667,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="63215104"/>
+        <c:crossAx val="64276352"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -810,11 +826,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="64307200"/>
-        <c:axId val="64308736"/>
+        <c:axId val="64328064"/>
+        <c:axId val="64329600"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="64307200"/>
+        <c:axId val="64328064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -834,12 +850,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="64308736"/>
+        <c:crossAx val="64329600"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="64308736"/>
+        <c:axId val="64329600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -850,7 +866,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="64307200"/>
+        <c:crossAx val="64328064"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1069,11 +1085,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="64545152"/>
-        <c:axId val="64546688"/>
+        <c:axId val="64538880"/>
+        <c:axId val="53477376"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="64545152"/>
+        <c:axId val="64538880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1093,12 +1109,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="64546688"/>
+        <c:crossAx val="53477376"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="64546688"/>
+        <c:axId val="53477376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1109,7 +1125,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="64545152"/>
+        <c:crossAx val="64538880"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1252,11 +1268,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="52015104"/>
-        <c:axId val="52016640"/>
+        <c:axId val="53531392"/>
+        <c:axId val="53532928"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="52015104"/>
+        <c:axId val="53531392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1276,12 +1292,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="52016640"/>
+        <c:crossAx val="53532928"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="52016640"/>
+        <c:axId val="53532928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1292,7 +1308,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="52015104"/>
+        <c:crossAx val="53531392"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1343,7 +1359,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1512,11 +1527,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="64491904"/>
-        <c:axId val="64493440"/>
+        <c:axId val="64832640"/>
+        <c:axId val="64834176"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="64491904"/>
+        <c:axId val="64832640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1536,12 +1551,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="64493440"/>
+        <c:crossAx val="64834176"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="64493440"/>
+        <c:axId val="64834176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1552,14 +1567,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="64491904"/>
+        <c:crossAx val="64832640"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1604,7 +1618,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1697,11 +1710,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="64584320"/>
-        <c:axId val="64586112"/>
+        <c:axId val="64851328"/>
+        <c:axId val="64853120"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="64584320"/>
+        <c:axId val="64851328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1721,12 +1734,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="64586112"/>
+        <c:crossAx val="64853120"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="64586112"/>
+        <c:axId val="64853120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1737,7 +1750,191 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="64584320"/>
+        <c:crossAx val="64851328"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-CA"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Axial Distance</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>B1 - B5</c:v>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>('Axial Distance'!$A$2,'Axial Distance'!$A$5)</c:f>
+              <c:numCache>
+                <c:formatCode>d\-mmm\-yy</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>42214</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>42215</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>('Axial Distance'!$D$2,'Axial Distance'!$D$5)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>40.57</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>39.96</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>F1 - F5</c:v>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>('Axial Distance'!$A$2,'Axial Distance'!$A$5)</c:f>
+              <c:numCache>
+                <c:formatCode>d\-mmm\-yy</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>42214</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>42215</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>('Axial Distance'!$D$3,'Axial Distance'!$D$6)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>39.93</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>39.81</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="66085248"/>
+        <c:axId val="66086784"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="66085248"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="d\-mmm\-yy" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr rot="-2100000" vert="horz"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="66086784"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="66086784"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="66085248"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2016,6 +2213,41 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>127000</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>355600</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2890,7 +3122,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozenSplit"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
     </sheetView>
@@ -3209,4 +3441,143 @@
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="G9" sqref="A4:G9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="4">
+        <v>42214</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2">
+        <v>40</v>
+      </c>
+      <c r="D2">
+        <v>40.57</v>
+      </c>
+      <c r="E2">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="F2">
+        <v>1.41</v>
+      </c>
+      <c r="G2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B3" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3">
+        <v>40</v>
+      </c>
+      <c r="D3">
+        <v>39.93</v>
+      </c>
+      <c r="E3">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="F3">
+        <v>0.17</v>
+      </c>
+      <c r="G3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="4">
+        <v>42215</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5">
+        <v>40</v>
+      </c>
+      <c r="D5">
+        <v>39.96</v>
+      </c>
+      <c r="E5">
+        <v>0.04</v>
+      </c>
+      <c r="F5">
+        <v>0.09</v>
+      </c>
+      <c r="G5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B6" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6">
+        <v>40</v>
+      </c>
+      <c r="D6">
+        <v>39.81</v>
+      </c>
+      <c r="E6">
+        <v>0.19</v>
+      </c>
+      <c r="F6">
+        <v>0.47</v>
+      </c>
+      <c r="G6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="4"/>
+      <c r="B8" s="2"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B9" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added lateral distance export.
</commit_message>
<xml_diff>
--- a/Log/ProstateBrachyQA Log.xlsx
+++ b/Log/ProstateBrachyQA Log.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="45" windowWidth="18195" windowHeight="12075" activeTab="5"/>
+    <workbookView xWindow="480" yWindow="45" windowWidth="18195" windowHeight="12075" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Phantom" sheetId="1" r:id="rId1"/>
@@ -13,13 +13,14 @@
     <sheet name="Axial Resolution" sheetId="4" r:id="rId4"/>
     <sheet name="Lateral Resolution" sheetId="5" r:id="rId5"/>
     <sheet name="Axial Distance" sheetId="6" r:id="rId6"/>
+    <sheet name="Lateral Distance" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="29">
   <si>
     <t>Phantom</t>
   </si>
@@ -94,6 +95,18 @@
   </si>
   <si>
     <t>F1 - F5</t>
+  </si>
+  <si>
+    <t>Lateral Distance</t>
+  </si>
+  <si>
+    <t>Proximal</t>
+  </si>
+  <si>
+    <t>Distal</t>
+  </si>
+  <si>
+    <t>Distance</t>
   </si>
 </sst>
 </file>
@@ -241,11 +254,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="63635840"/>
-        <c:axId val="63637376"/>
+        <c:axId val="61412096"/>
+        <c:axId val="61413632"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="63635840"/>
+        <c:axId val="61412096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -265,12 +278,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="63637376"/>
+        <c:crossAx val="61413632"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="63637376"/>
+        <c:axId val="61413632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -281,13 +294,345 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="63635840"/>
+        <c:crossAx val="61412096"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart10.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-CA"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Lateral Distance (Axial)</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Proximal</c:v>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>('Lateral Distance'!$A$3,'Lateral Distance'!$A$6)</c:f>
+              <c:numCache>
+                <c:formatCode>d\-mmm\-yy</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>42214</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>42215</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>('Lateral Distance'!$D$3,'Lateral Distance'!$D$6)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>41.28</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>40.86</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Distal</c:v>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>('Lateral Distance'!$A$3,'Lateral Distance'!$A$6)</c:f>
+              <c:numCache>
+                <c:formatCode>d\-mmm\-yy</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>42214</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>42215</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>('Lateral Distance'!$D$4,'Lateral Distance'!$D$7)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>40.76</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>40.97</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="66817408"/>
+        <c:axId val="66831488"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="66817408"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="d\-mmm\-yy" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr rot="-2100000" vert="horz"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="66831488"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="66831488"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="66817408"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart11.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-CA"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Lateral Distance (Longitudinal)</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Distance</c:v>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>('Lateral Distance'!$A$3,'Lateral Distance'!$A$6)</c:f>
+              <c:numCache>
+                <c:formatCode>d\-mmm\-yy</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>42214</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>42215</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>('Lateral Distance'!$J$3,'Lateral Distance'!$J$6)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>40.65</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>39.58</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="66843776"/>
+        <c:axId val="66845312"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="66843776"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="d\-mmm\-yy" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr rot="-2100000" vert="horz"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="66845312"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="66845312"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="66843776"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -428,11 +773,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="63699968"/>
-        <c:axId val="64254720"/>
+        <c:axId val="63184256"/>
+        <c:axId val="63206528"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="63699968"/>
+        <c:axId val="63184256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -452,12 +797,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="64254720"/>
+        <c:crossAx val="63206528"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="64254720"/>
+        <c:axId val="63206528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -468,7 +813,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="63699968"/>
+        <c:crossAx val="63184256"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -627,11 +972,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="64276352"/>
-        <c:axId val="64277888"/>
+        <c:axId val="63232256"/>
+        <c:axId val="63238144"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="64276352"/>
+        <c:axId val="63232256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -651,12 +996,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="64277888"/>
+        <c:crossAx val="63238144"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="64277888"/>
+        <c:axId val="63238144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -667,7 +1012,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="64276352"/>
+        <c:crossAx val="63232256"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -826,11 +1171,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="64328064"/>
-        <c:axId val="64329600"/>
+        <c:axId val="65385216"/>
+        <c:axId val="65386752"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="64328064"/>
+        <c:axId val="65385216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -850,12 +1195,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="64329600"/>
+        <c:crossAx val="65386752"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="64329600"/>
+        <c:axId val="65386752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -866,7 +1211,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="64328064"/>
+        <c:crossAx val="65385216"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1085,11 +1430,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="64538880"/>
-        <c:axId val="53477376"/>
+        <c:axId val="66644608"/>
+        <c:axId val="60952960"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="64538880"/>
+        <c:axId val="66644608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1109,12 +1454,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="53477376"/>
+        <c:crossAx val="60952960"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="53477376"/>
+        <c:axId val="60952960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1125,7 +1470,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="64538880"/>
+        <c:crossAx val="66644608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1268,11 +1613,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="53531392"/>
-        <c:axId val="53532928"/>
+        <c:axId val="61060224"/>
+        <c:axId val="61061760"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="53531392"/>
+        <c:axId val="61060224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1292,12 +1637,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="53532928"/>
+        <c:crossAx val="61061760"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="53532928"/>
+        <c:axId val="61061760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1308,7 +1653,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="53531392"/>
+        <c:crossAx val="61060224"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1527,11 +1872,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="64832640"/>
-        <c:axId val="64834176"/>
+        <c:axId val="66668032"/>
+        <c:axId val="66669568"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="64832640"/>
+        <c:axId val="66668032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1551,12 +1896,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="64834176"/>
+        <c:crossAx val="66669568"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="64834176"/>
+        <c:axId val="66669568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1567,7 +1912,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="64832640"/>
+        <c:crossAx val="66668032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1710,11 +2055,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="64851328"/>
-        <c:axId val="64853120"/>
+        <c:axId val="66691072"/>
+        <c:axId val="66692608"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="64851328"/>
+        <c:axId val="66691072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1734,12 +2079,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="64853120"/>
+        <c:crossAx val="66692608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="64853120"/>
+        <c:axId val="66692608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1750,7 +2095,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="64851328"/>
+        <c:crossAx val="66691072"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1801,7 +2146,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1894,11 +2238,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="66085248"/>
-        <c:axId val="66086784"/>
+        <c:axId val="66872064"/>
+        <c:axId val="66873600"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="66085248"/>
+        <c:axId val="66872064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1918,12 +2262,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="66086784"/>
+        <c:crossAx val="66873600"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="66086784"/>
+        <c:axId val="66873600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1934,14 +2278,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="66085248"/>
+        <c:crossAx val="66872064"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2256,6 +2599,71 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>127000</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>117475</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>127000</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>98425</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -2778,7 +3186,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
+      <selection pane="bottomLeft" activeCell="A7" sqref="A7:M16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3447,7 +3855,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
       <selection pane="bottomLeft" activeCell="G9" sqref="A4:G9"/>
     </sheetView>
@@ -3580,4 +3988,223 @@
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="6.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
+      <c r="K1" s="5"/>
+      <c r="L1" s="5"/>
+    </row>
+    <row r="2" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" s="4">
+        <v>42214</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3">
+        <v>40</v>
+      </c>
+      <c r="D3">
+        <v>41.28</v>
+      </c>
+      <c r="E3">
+        <v>1.28</v>
+      </c>
+      <c r="F3">
+        <v>3.16</v>
+      </c>
+      <c r="G3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="I3">
+        <v>40</v>
+      </c>
+      <c r="J3">
+        <v>40.65</v>
+      </c>
+      <c r="K3">
+        <v>0.65</v>
+      </c>
+      <c r="L3">
+        <v>1.61</v>
+      </c>
+      <c r="M3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" s="4"/>
+      <c r="B4" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4">
+        <v>40</v>
+      </c>
+      <c r="D4">
+        <v>40.76</v>
+      </c>
+      <c r="E4">
+        <v>0.76</v>
+      </c>
+      <c r="F4">
+        <v>1.87</v>
+      </c>
+      <c r="G4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H4" s="2"/>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B5" s="2"/>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" s="4">
+        <v>42215</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6">
+        <v>40</v>
+      </c>
+      <c r="D6">
+        <v>40.86</v>
+      </c>
+      <c r="E6">
+        <v>0.86</v>
+      </c>
+      <c r="F6">
+        <v>2.13</v>
+      </c>
+      <c r="G6" t="s">
+        <v>6</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="I6">
+        <v>40</v>
+      </c>
+      <c r="J6">
+        <v>39.58</v>
+      </c>
+      <c r="K6">
+        <v>0.42</v>
+      </c>
+      <c r="L6">
+        <v>1.05</v>
+      </c>
+      <c r="M6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" s="4"/>
+      <c r="B7" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7">
+        <v>40</v>
+      </c>
+      <c r="D7">
+        <v>40.97</v>
+      </c>
+      <c r="E7">
+        <v>0.97</v>
+      </c>
+      <c r="F7">
+        <v>2.38</v>
+      </c>
+      <c r="G7" t="s">
+        <v>6</v>
+      </c>
+      <c r="H7" s="2"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B8" s="2"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B1:G1"/>
+    <mergeCell ref="H1:L1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added area test export.
</commit_message>
<xml_diff>
--- a/Log/ProstateBrachyQA Log.xlsx
+++ b/Log/ProstateBrachyQA Log.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="45" windowWidth="18195" windowHeight="12075" activeTab="6"/>
+    <workbookView xWindow="480" yWindow="45" windowWidth="18195" windowHeight="12075" firstSheet="1" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Phantom" sheetId="1" r:id="rId1"/>
@@ -14,13 +14,14 @@
     <sheet name="Lateral Resolution" sheetId="5" r:id="rId5"/>
     <sheet name="Axial Distance" sheetId="6" r:id="rId6"/>
     <sheet name="Lateral Distance" sheetId="7" r:id="rId7"/>
+    <sheet name="Area" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="32">
   <si>
     <t>Phantom</t>
   </si>
@@ -107,6 +108,15 @@
   </si>
   <si>
     <t>Distance</t>
+  </si>
+  <si>
+    <t>Area</t>
+  </si>
+  <si>
+    <t>Known (cm^2)</t>
+  </si>
+  <si>
+    <t>Measured (cm^2)</t>
   </si>
 </sst>
 </file>
@@ -254,11 +264,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="61412096"/>
-        <c:axId val="61413632"/>
+        <c:axId val="65234816"/>
+        <c:axId val="65236352"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="61412096"/>
+        <c:axId val="65234816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -278,12 +288,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="61413632"/>
+        <c:crossAx val="65236352"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="61413632"/>
+        <c:axId val="65236352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -294,7 +304,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="61412096"/>
+        <c:crossAx val="65234816"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -345,7 +355,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -438,11 +447,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="66817408"/>
-        <c:axId val="66831488"/>
+        <c:axId val="69964544"/>
+        <c:axId val="69966080"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="66817408"/>
+        <c:axId val="69964544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -462,12 +471,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="66831488"/>
+        <c:crossAx val="69966080"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="66831488"/>
+        <c:axId val="69966080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -478,14 +487,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="66817408"/>
+        <c:crossAx val="69964544"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -530,7 +538,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -585,11 +592,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="66843776"/>
-        <c:axId val="66845312"/>
+        <c:axId val="69814528"/>
+        <c:axId val="69824512"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="66843776"/>
+        <c:axId val="69814528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -609,12 +616,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="66845312"/>
+        <c:crossAx val="69824512"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="66845312"/>
+        <c:axId val="69824512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -625,7 +632,161 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="66843776"/>
+        <c:crossAx val="69814528"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart12.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-CA"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Area</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Area!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Measured (cm^2)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Area!$A$2:$A$3</c:f>
+              <c:numCache>
+                <c:formatCode>d\-mmm\-yy</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>42214</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>42215</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Area!$C$2:$C$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>5.3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7.23</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="69886336"/>
+        <c:axId val="69887872"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="69886336"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="d\-mmm\-yy" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr rot="-2100000" vert="horz"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="69887872"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="69887872"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="69886336"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -677,6 +838,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -773,11 +935,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="63184256"/>
-        <c:axId val="63206528"/>
+        <c:axId val="68137728"/>
+        <c:axId val="68139264"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="63184256"/>
+        <c:axId val="68137728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -797,12 +959,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="63206528"/>
+        <c:crossAx val="68139264"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="63206528"/>
+        <c:axId val="68139264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -813,13 +975,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="63184256"/>
+        <c:crossAx val="68137728"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -864,6 +1027,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -972,11 +1136,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="63232256"/>
-        <c:axId val="63238144"/>
+        <c:axId val="68169088"/>
+        <c:axId val="68174976"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="63232256"/>
+        <c:axId val="68169088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -996,12 +1160,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="63238144"/>
+        <c:crossAx val="68174976"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="63238144"/>
+        <c:axId val="68174976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1012,13 +1176,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="63232256"/>
+        <c:crossAx val="68169088"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1063,6 +1228,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1171,11 +1337,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="65385216"/>
-        <c:axId val="65386752"/>
+        <c:axId val="68208512"/>
+        <c:axId val="68210048"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="65385216"/>
+        <c:axId val="68208512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1195,12 +1361,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="65386752"/>
+        <c:crossAx val="68210048"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="65386752"/>
+        <c:axId val="68210048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1211,13 +1377,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="65385216"/>
+        <c:crossAx val="68208512"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1262,6 +1429,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1430,11 +1598,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="66644608"/>
-        <c:axId val="60952960"/>
+        <c:axId val="68296704"/>
+        <c:axId val="68298240"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="66644608"/>
+        <c:axId val="68296704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1454,12 +1622,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="60952960"/>
+        <c:crossAx val="68298240"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="60952960"/>
+        <c:axId val="68298240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1470,13 +1638,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="66644608"/>
+        <c:crossAx val="68296704"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1521,6 +1690,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1613,11 +1783,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="61060224"/>
-        <c:axId val="61061760"/>
+        <c:axId val="68309760"/>
+        <c:axId val="68311296"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="61060224"/>
+        <c:axId val="68309760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1637,12 +1807,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="61061760"/>
+        <c:crossAx val="68311296"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="61061760"/>
+        <c:axId val="68311296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1653,13 +1823,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="61060224"/>
+        <c:crossAx val="68309760"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1872,11 +2043,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="66668032"/>
-        <c:axId val="66669568"/>
+        <c:axId val="68580096"/>
+        <c:axId val="68581632"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="66668032"/>
+        <c:axId val="68580096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1896,12 +2067,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="66669568"/>
+        <c:crossAx val="68581632"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="66669568"/>
+        <c:axId val="68581632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1912,7 +2083,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="66668032"/>
+        <c:crossAx val="68580096"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2055,11 +2226,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="66691072"/>
-        <c:axId val="66692608"/>
+        <c:axId val="68606976"/>
+        <c:axId val="68608768"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="66691072"/>
+        <c:axId val="68606976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2079,12 +2250,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="66692608"/>
+        <c:crossAx val="68608768"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="66692608"/>
+        <c:axId val="68608768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2095,7 +2266,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="66691072"/>
+        <c:crossAx val="68606976"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2238,11 +2409,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="66872064"/>
-        <c:axId val="66873600"/>
+        <c:axId val="68540288"/>
+        <c:axId val="68541824"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="66872064"/>
+        <c:axId val="68540288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2262,12 +2433,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="66873600"/>
+        <c:crossAx val="68541824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="66873600"/>
+        <c:axId val="68541824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2278,7 +2449,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="66872064"/>
+        <c:crossAx val="68540288"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2664,6 +2835,41 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing8.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>127000</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>527050</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -3994,7 +4200,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozenSplit"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
     </sheetView>
@@ -4207,4 +4413,89 @@
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="8.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="4">
+        <v>42214</v>
+      </c>
+      <c r="B2">
+        <v>7</v>
+      </c>
+      <c r="C2">
+        <v>5.3</v>
+      </c>
+      <c r="D2">
+        <v>1.7</v>
+      </c>
+      <c r="E2">
+        <v>27.67</v>
+      </c>
+      <c r="F2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="4">
+        <v>42215</v>
+      </c>
+      <c r="B3">
+        <v>7</v>
+      </c>
+      <c r="C3">
+        <v>7.23</v>
+      </c>
+      <c r="D3">
+        <v>0.23</v>
+      </c>
+      <c r="E3">
+        <v>3.29</v>
+      </c>
+      <c r="F3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Removed baseline from grayscale and depth test charts.
</commit_message>
<xml_diff>
--- a/Log/ProstateBrachyQA Log.xlsx
+++ b/Log/ProstateBrachyQA Log.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="45" windowWidth="18195" windowHeight="12075" firstSheet="1" activeTab="7"/>
+    <workbookView xWindow="480" yWindow="45" windowWidth="18195" windowHeight="12075" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Phantom" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="32">
   <si>
     <t>Phantom</t>
   </si>
@@ -264,11 +264,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="65234816"/>
-        <c:axId val="65236352"/>
+        <c:axId val="68642688"/>
+        <c:axId val="68644224"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="65234816"/>
+        <c:axId val="68642688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -288,12 +288,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="65236352"/>
+        <c:crossAx val="68644224"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="65236352"/>
+        <c:axId val="68644224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -304,7 +304,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="65234816"/>
+        <c:crossAx val="68642688"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -447,11 +447,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="69964544"/>
-        <c:axId val="69966080"/>
+        <c:axId val="69818624"/>
+        <c:axId val="69836800"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="69964544"/>
+        <c:axId val="69818624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -471,12 +471,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="69966080"/>
+        <c:crossAx val="69836800"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="69966080"/>
+        <c:axId val="69836800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -487,7 +487,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="69964544"/>
+        <c:crossAx val="69818624"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -592,11 +592,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="69814528"/>
-        <c:axId val="69824512"/>
+        <c:axId val="71766016"/>
+        <c:axId val="71767552"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="69814528"/>
+        <c:axId val="71766016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -616,12 +616,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="69824512"/>
+        <c:crossAx val="71767552"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="69824512"/>
+        <c:axId val="71767552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -632,7 +632,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="69814528"/>
+        <c:crossAx val="71766016"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -683,7 +683,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -746,11 +745,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="69886336"/>
-        <c:axId val="69887872"/>
+        <c:axId val="71911296"/>
+        <c:axId val="71912832"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="69886336"/>
+        <c:axId val="71911296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -770,12 +769,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="69887872"/>
+        <c:crossAx val="71912832"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="69887872"/>
+        <c:axId val="71912832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -786,14 +785,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="69886336"/>
+        <c:crossAx val="71911296"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -838,7 +836,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -852,22 +849,25 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Grayscale!$B$1</c:f>
+              <c:f>Grayscale!$C$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Baseline (mm)</c:v>
+                  <c:v>Current (mm)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>Grayscale!$A$2</c:f>
+              <c:f>Grayscale!$A$2:$A$3</c:f>
               <c:numCache>
                 <c:formatCode>d\-mmm\-yy</c:formatCode>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>42214</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>42215</c:v>
                 </c:pt>
               </c:numCache>
@@ -875,52 +875,15 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Grayscale!$B$2</c:f>
+              <c:f>Grayscale!$C$2:$C$3</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>10.7</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Grayscale!$C$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Current (mm)</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:xVal>
-            <c:numRef>
-              <c:f>Grayscale!$A$2</c:f>
-              <c:numCache>
-                <c:formatCode>d\-mmm\-yy</c:formatCode>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>42215</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Grayscale!$C$2</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="1"/>
+                <c:ptCount val="2"/>
                 <c:pt idx="0">
                   <c:v>11.06</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>14.75</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -935,11 +898,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="68137728"/>
-        <c:axId val="68139264"/>
+        <c:axId val="68857856"/>
+        <c:axId val="68859392"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="68137728"/>
+        <c:axId val="68857856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -959,12 +922,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="68139264"/>
+        <c:crossAx val="68859392"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="68139264"/>
+        <c:axId val="68859392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -975,14 +938,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="68137728"/>
+        <c:crossAx val="68857856"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1041,11 +1003,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Depth!$B$2</c:f>
+              <c:f>Depth!$C$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Baseline (mm)</c:v>
+                  <c:v>Current (mm)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1057,53 +1019,7 @@
                 <c:formatCode>d\-mmm\-yy</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>42215</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>42215</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Depth!$B$3:$B$4</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>75.3</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>75.3</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Depth!$C$2</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Current (mm)</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:xVal>
-            <c:numRef>
-              <c:f>Depth!$A$3:$A$4</c:f>
-              <c:numCache>
-                <c:formatCode>d\-mmm\-yy</c:formatCode>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>42215</c:v>
+                  <c:v>42214</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>42215</c:v>
@@ -1121,7 +1037,7 @@
                   <c:v>85.42</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>85.42</c:v>
+                  <c:v>80.180000000000007</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1136,11 +1052,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="68169088"/>
-        <c:axId val="68174976"/>
+        <c:axId val="69613440"/>
+        <c:axId val="69614976"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="68169088"/>
+        <c:axId val="69613440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1160,12 +1076,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="68174976"/>
+        <c:crossAx val="69614976"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="68174976"/>
+        <c:axId val="69614976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1176,7 +1092,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="68169088"/>
+        <c:crossAx val="69613440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1242,11 +1158,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Depth!$E$2</c:f>
+              <c:f>Depth!$F$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Baseline (mm)</c:v>
+                  <c:v>Current (mm)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1258,53 +1174,7 @@
                 <c:formatCode>d\-mmm\-yy</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>42215</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>42215</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Depth!$E$3:$E$4</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>78.8</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>78.8</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Depth!$F$2</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Current (mm)</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:xVal>
-            <c:numRef>
-              <c:f>Depth!$A$3:$A$4</c:f>
-              <c:numCache>
-                <c:formatCode>d\-mmm\-yy</c:formatCode>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>42215</c:v>
+                  <c:v>42214</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>42215</c:v>
@@ -1322,7 +1192,7 @@
                   <c:v>79.2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>79.2</c:v>
+                  <c:v>63.94</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1337,11 +1207,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="68208512"/>
-        <c:axId val="68210048"/>
+        <c:axId val="69643648"/>
+        <c:axId val="69653632"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="68208512"/>
+        <c:axId val="69643648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1361,12 +1231,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="68210048"/>
+        <c:crossAx val="69653632"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="68210048"/>
+        <c:axId val="69653632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1377,7 +1247,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="68208512"/>
+        <c:crossAx val="69643648"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1429,7 +1299,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1598,11 +1467,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="68296704"/>
-        <c:axId val="68298240"/>
+        <c:axId val="71030272"/>
+        <c:axId val="71031808"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="68296704"/>
+        <c:axId val="71030272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1622,12 +1491,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="68298240"/>
+        <c:crossAx val="71031808"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="68298240"/>
+        <c:axId val="71031808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1638,14 +1507,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="68296704"/>
+        <c:crossAx val="71030272"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1690,7 +1558,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1783,11 +1650,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="68309760"/>
-        <c:axId val="68311296"/>
+        <c:axId val="71065600"/>
+        <c:axId val="71067136"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="68309760"/>
+        <c:axId val="71065600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1807,12 +1674,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="68311296"/>
+        <c:crossAx val="71067136"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="68311296"/>
+        <c:axId val="71067136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1823,14 +1690,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="68309760"/>
+        <c:crossAx val="71065600"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2043,11 +1909,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="68580096"/>
-        <c:axId val="68581632"/>
+        <c:axId val="71123328"/>
+        <c:axId val="71124864"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="68580096"/>
+        <c:axId val="71123328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2067,12 +1933,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="68581632"/>
+        <c:crossAx val="71124864"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="68581632"/>
+        <c:axId val="71124864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2083,7 +1949,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="68580096"/>
+        <c:crossAx val="71123328"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2226,11 +2092,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="68606976"/>
-        <c:axId val="68608768"/>
+        <c:axId val="71158400"/>
+        <c:axId val="71164288"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="68606976"/>
+        <c:axId val="71158400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2250,12 +2116,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="68608768"/>
+        <c:crossAx val="71164288"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="68608768"/>
+        <c:axId val="71164288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2266,7 +2132,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="68606976"/>
+        <c:crossAx val="71158400"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2409,11 +2275,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="68540288"/>
-        <c:axId val="68541824"/>
+        <c:axId val="69785088"/>
+        <c:axId val="69786624"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="68540288"/>
+        <c:axId val="69785088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2433,12 +2299,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="68541824"/>
+        <c:crossAx val="69786624"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="68541824"/>
+        <c:axId val="69786624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2449,7 +2315,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="68540288"/>
+        <c:crossAx val="69785088"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2511,13 +2377,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>127000</xdr:colOff>
-      <xdr:row>3</xdr:row>
+      <xdr:row>4</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>203200</xdr:colOff>
-      <xdr:row>17</xdr:row>
+      <xdr:row>18</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -3219,7 +3085,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" sqref="A1:A1048576"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3246,7 +3112,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
-        <v>42215</v>
+        <v>42214</v>
       </c>
       <c r="B2">
         <v>10.7</v>
@@ -3259,7 +3125,18 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="4"/>
+      <c r="A3" s="4">
+        <v>42215</v>
+      </c>
+      <c r="B3">
+        <v>10.7</v>
+      </c>
+      <c r="C3">
+        <v>14.75</v>
+      </c>
+      <c r="D3" t="s">
+        <v>9</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3272,9 +3149,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="G30" sqref="G30"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3325,7 +3202,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
-        <v>42215</v>
+        <v>42214</v>
       </c>
       <c r="B3">
         <v>75.3</v>
@@ -3354,19 +3231,19 @@
         <v>75.3</v>
       </c>
       <c r="C4">
-        <v>85.42</v>
+        <v>80.180000000000007</v>
       </c>
       <c r="D4" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E4">
         <v>78.8</v>
       </c>
       <c r="F4">
-        <v>79.2</v>
+        <v>63.94</v>
       </c>
       <c r="G4" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -4419,7 +4296,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
     </sheetView>

</xml_diff>

<commit_message>
Added image export to grayscale test.
- Image is saved to Log/Images folder
- Link to image is placed in excel sheet
- Cell comment is added so that image preview shows on mouse hover
</commit_message>
<xml_diff>
--- a/Log/ProstateBrachyQA Log.xlsx
+++ b/Log/ProstateBrachyQA Log.xlsx
@@ -4,11 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="45" windowWidth="18195" windowHeight="12075" activeTab="2"/>
+    <workbookView xWindow="480" yWindow="45" windowWidth="18195" windowHeight="12075" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Phantom" sheetId="1" r:id="rId1"/>
-    <sheet name="Grayscale" sheetId="2" r:id="rId2"/>
+    <sheet name="Grayscale" sheetId="9" r:id="rId2"/>
     <sheet name="Depth" sheetId="3" r:id="rId3"/>
     <sheet name="Axial Resolution" sheetId="4" r:id="rId4"/>
     <sheet name="Lateral Resolution" sheetId="5" r:id="rId5"/>
@@ -20,8 +20,42 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Poon, Justin</author>
+  </authors>
+  <commentList>
+    <comment ref="E2" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Poon, Justin:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="34">
   <si>
     <t>Phantom</t>
   </si>
@@ -118,12 +152,18 @@
   <si>
     <t>Measured (cm^2)</t>
   </si>
+  <si>
+    <t>Image</t>
+  </si>
+  <si>
+    <t>View Image</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -138,6 +178,27 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -163,18 +224,21 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="15" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -264,11 +328,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="68642688"/>
-        <c:axId val="68644224"/>
+        <c:axId val="61281024"/>
+        <c:axId val="61282560"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="68642688"/>
+        <c:axId val="61281024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -288,12 +352,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="68644224"/>
+        <c:crossAx val="61282560"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="68644224"/>
+        <c:axId val="61282560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -304,7 +368,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="68642688"/>
+        <c:crossAx val="61281024"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -447,11 +511,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="69818624"/>
-        <c:axId val="69836800"/>
+        <c:axId val="63523840"/>
+        <c:axId val="63558400"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="69818624"/>
+        <c:axId val="63523840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -471,12 +535,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="69836800"/>
+        <c:crossAx val="63558400"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="69836800"/>
+        <c:axId val="63558400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -487,7 +551,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="69818624"/>
+        <c:crossAx val="63523840"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -592,11 +656,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="71766016"/>
-        <c:axId val="71767552"/>
+        <c:axId val="63386368"/>
+        <c:axId val="63387904"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="71766016"/>
+        <c:axId val="63386368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -616,12 +680,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="71767552"/>
+        <c:crossAx val="63387904"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="71767552"/>
+        <c:axId val="63387904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -632,7 +696,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="71766016"/>
+        <c:crossAx val="63386368"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -745,11 +809,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="71911296"/>
-        <c:axId val="71912832"/>
+        <c:axId val="63412864"/>
+        <c:axId val="63435136"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="71911296"/>
+        <c:axId val="63412864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -769,12 +833,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="71912832"/>
+        <c:crossAx val="63435136"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="71912832"/>
+        <c:axId val="63435136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -785,7 +849,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="71911296"/>
+        <c:crossAx val="63412864"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -836,6 +900,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -860,30 +925,24 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>Grayscale!$A$2:$A$3</c:f>
+              <c:f>Grayscale!$A$2</c:f>
               <c:numCache>
                 <c:formatCode>d\-mmm\-yy</c:formatCode>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>42214</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>42215</c:v>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>42216</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Grayscale!$C$2:$C$3</c:f>
+              <c:f>Grayscale!$C$2</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="2"/>
+                <c:ptCount val="1"/>
                 <c:pt idx="0">
                   <c:v>11.06</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>14.75</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -898,11 +957,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="68857856"/>
-        <c:axId val="68859392"/>
+        <c:axId val="80260480"/>
+        <c:axId val="79760000"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="68857856"/>
+        <c:axId val="80260480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -922,12 +981,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="68859392"/>
+        <c:crossAx val="79760000"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="68859392"/>
+        <c:axId val="79760000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -938,13 +997,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="68857856"/>
+        <c:crossAx val="80260480"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1052,11 +1112,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="69613440"/>
-        <c:axId val="69614976"/>
+        <c:axId val="50924160"/>
+        <c:axId val="50983296"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="69613440"/>
+        <c:axId val="50924160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1076,12 +1136,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="69614976"/>
+        <c:crossAx val="50983296"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="69614976"/>
+        <c:axId val="50983296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1092,7 +1152,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="69613440"/>
+        <c:crossAx val="50924160"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1207,11 +1267,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="69643648"/>
-        <c:axId val="69653632"/>
+        <c:axId val="51048832"/>
+        <c:axId val="51050368"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="69643648"/>
+        <c:axId val="51048832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1231,12 +1291,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="69653632"/>
+        <c:crossAx val="51050368"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="69653632"/>
+        <c:axId val="51050368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1247,7 +1307,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="69643648"/>
+        <c:crossAx val="51048832"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1467,11 +1527,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="71030272"/>
-        <c:axId val="71031808"/>
+        <c:axId val="62104320"/>
+        <c:axId val="62105856"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="71030272"/>
+        <c:axId val="62104320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1491,12 +1551,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="71031808"/>
+        <c:crossAx val="62105856"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="71031808"/>
+        <c:axId val="62105856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1507,7 +1567,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="71030272"/>
+        <c:crossAx val="62104320"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1650,11 +1710,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="71065600"/>
-        <c:axId val="71067136"/>
+        <c:axId val="63447808"/>
+        <c:axId val="63449344"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="71065600"/>
+        <c:axId val="63447808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1674,12 +1734,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="71067136"/>
+        <c:crossAx val="63449344"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="71067136"/>
+        <c:axId val="63449344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1690,7 +1750,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="71065600"/>
+        <c:crossAx val="63447808"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1909,11 +1969,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="71123328"/>
-        <c:axId val="71124864"/>
+        <c:axId val="63300736"/>
+        <c:axId val="63302272"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="71123328"/>
+        <c:axId val="63300736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1933,12 +1993,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="71124864"/>
+        <c:crossAx val="63302272"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="71124864"/>
+        <c:axId val="63302272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1949,7 +2009,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="71123328"/>
+        <c:crossAx val="63300736"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2092,11 +2152,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="71158400"/>
-        <c:axId val="71164288"/>
+        <c:axId val="63178240"/>
+        <c:axId val="63179776"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="71158400"/>
+        <c:axId val="63178240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2116,12 +2176,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="71164288"/>
+        <c:crossAx val="63179776"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="71164288"/>
+        <c:axId val="63179776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2132,7 +2192,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="71158400"/>
+        <c:crossAx val="63178240"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2275,11 +2335,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="69785088"/>
-        <c:axId val="69786624"/>
+        <c:axId val="63209856"/>
+        <c:axId val="63211392"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="69785088"/>
+        <c:axId val="63209856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2299,12 +2359,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="69786624"/>
+        <c:crossAx val="63211392"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="69786624"/>
+        <c:axId val="63211392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2315,7 +2375,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="69785088"/>
+        <c:crossAx val="63209856"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2377,13 +2437,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>127000</xdr:colOff>
-      <xdr:row>4</xdr:row>
+      <xdr:row>3</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>203200</xdr:colOff>
-      <xdr:row>18</xdr:row>
+      <xdr:colOff>50800</xdr:colOff>
+      <xdr:row>17</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -3080,12 +3140,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3094,9 +3154,10 @@
     <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>2</v>
       </c>
@@ -3109,10 +3170,13 @@
       <c r="D1" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
-        <v>42214</v>
+        <v>42216</v>
       </c>
       <c r="B2">
         <v>10.7</v>
@@ -3123,25 +3187,18 @@
       <c r="D2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="4">
-        <v>42215</v>
-      </c>
-      <c r="B3">
-        <v>10.7</v>
-      </c>
-      <c r="C3">
-        <v>14.75</v>
-      </c>
-      <c r="D3" t="s">
-        <v>9</v>
+      <c r="E2" s="6" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E2" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
-  <drawing r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -3149,7 +3206,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozenSplit"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
     </sheetView>

</xml_diff>

<commit_message>
Added image export to lat. res, axial/lat distance, and area tests.
</commit_message>
<xml_diff>
--- a/Log/ProstateBrachyQA Log.xlsx
+++ b/Log/ProstateBrachyQA Log.xlsx
@@ -4,13 +4,17 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="45" windowWidth="18195" windowHeight="12075" firstSheet="1" activeTab="3"/>
+    <workbookView xWindow="480" yWindow="45" windowWidth="18195" windowHeight="12075" firstSheet="1" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Phantom" sheetId="1" r:id="rId1"/>
-    <sheet name="Grayscale" sheetId="9" r:id="rId2"/>
+    <sheet name="Grayscale" sheetId="2" r:id="rId2"/>
     <sheet name="Depth" sheetId="3" r:id="rId3"/>
-    <sheet name="Axial Resolution" sheetId="10" r:id="rId4"/>
+    <sheet name="Axial Resolution" sheetId="4" r:id="rId4"/>
+    <sheet name="Lateral Resolution" sheetId="5" r:id="rId5"/>
+    <sheet name="Axial Distance" sheetId="6" r:id="rId6"/>
+    <sheet name="Lateral Distance" sheetId="7" r:id="rId7"/>
+    <sheet name="Area" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
@@ -166,8 +170,192 @@
 </comments>
 </file>
 
+<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Poon, Justin</author>
+  </authors>
+  <commentList>
+    <comment ref="H3" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Poon, Justin:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="O3" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Poon, Justin:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Poon, Justin</author>
+  </authors>
+  <commentList>
+    <comment ref="H2" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Poon, Justin:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments6.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Poon, Justin</author>
+  </authors>
+  <commentList>
+    <comment ref="H3" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Poon, Justin:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="O3" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Poon, Justin:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments7.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Poon, Justin</author>
+  </authors>
+  <commentList>
+    <comment ref="G2" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Poon, Justin:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="34">
   <si>
     <t>Phantom</t>
   </si>
@@ -187,19 +375,22 @@
     <t>Result</t>
   </si>
   <si>
+    <t>Image</t>
+  </si>
+  <si>
     <t>PASS</t>
+  </si>
+  <si>
+    <t>View Image</t>
   </si>
   <si>
     <t>Axial Plane</t>
   </si>
   <si>
-    <t>FAIL</t>
+    <t>Longitudinal Plane</t>
   </si>
   <si>
-    <t>Image</t>
-  </si>
-  <si>
-    <t>View Image</t>
+    <t>FAIL</t>
   </si>
   <si>
     <t>Axial Resolution</t>
@@ -209,9 +400,6 @@
   </si>
   <si>
     <t>Diff (%)</t>
-  </si>
-  <si>
-    <t>Longitudinal Plane</t>
   </si>
   <si>
     <t>Proximal (B1)</t>
@@ -230,6 +418,45 @@
   </si>
   <si>
     <t>Filament 6</t>
+  </si>
+  <si>
+    <t>Lateral Resolution</t>
+  </si>
+  <si>
+    <t>Axial Distance</t>
+  </si>
+  <si>
+    <t>Known (mm)</t>
+  </si>
+  <si>
+    <t>Measured (mm)</t>
+  </si>
+  <si>
+    <t>B1 - B5</t>
+  </si>
+  <si>
+    <t>F1 - F5</t>
+  </si>
+  <si>
+    <t>Lateral Distance</t>
+  </si>
+  <si>
+    <t>Proximal</t>
+  </si>
+  <si>
+    <t>Distal</t>
+  </si>
+  <si>
+    <t>Distance</t>
+  </si>
+  <si>
+    <t>Area</t>
+  </si>
+  <si>
+    <t>Known (cm^2)</t>
+  </si>
+  <si>
+    <t>Measured (cm^2)</t>
   </si>
 </sst>
 </file>
@@ -401,11 +628,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="53788032"/>
-        <c:axId val="53793920"/>
+        <c:axId val="63386752"/>
+        <c:axId val="63388288"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="53788032"/>
+        <c:axId val="63386752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -425,12 +652,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="53793920"/>
+        <c:crossAx val="63388288"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="53793920"/>
+        <c:axId val="63388288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -441,13 +668,476 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="53788032"/>
+        <c:crossAx val="63386752"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart10.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-CA"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Lateral Distance (Axial)</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Proximal</c:v>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Lateral Distance'!$A$3</c:f>
+              <c:numCache>
+                <c:formatCode>d\-mmm\-yy</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>42216</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Lateral Distance'!$D$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>40.86</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Distal</c:v>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Lateral Distance'!$A$3</c:f>
+              <c:numCache>
+                <c:formatCode>d\-mmm\-yy</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>42216</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Lateral Distance'!$D$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>40.97</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="76581120"/>
+        <c:axId val="76587008"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="76581120"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="d\-mmm\-yy" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr rot="-2100000" vert="horz"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="76587008"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="76587008"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="76581120"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart11.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-CA"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Lateral Distance (Longitudinal)</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Distance</c:v>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Lateral Distance'!$A$3</c:f>
+              <c:numCache>
+                <c:formatCode>d\-mmm\-yy</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>42216</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Lateral Distance'!$K$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>39.58</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="76607488"/>
+        <c:axId val="76609024"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="76607488"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="d\-mmm\-yy" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr rot="-2100000" vert="horz"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="76609024"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="76609024"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="76607488"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart12.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-CA"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Area</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Area!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Measured (cm^2)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Area!$A$2</c:f>
+              <c:numCache>
+                <c:formatCode>d\-mmm\-yy</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>42216</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Area!$C$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>7.23</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="91556864"/>
+        <c:axId val="89803008"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="91556864"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="d\-mmm\-yy" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr rot="-2100000" vert="horz"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="89803008"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="89803008"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="91556864"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -548,11 +1238,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="64350080"/>
-        <c:axId val="64351616"/>
+        <c:axId val="65372160"/>
+        <c:axId val="65373696"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="64350080"/>
+        <c:axId val="65372160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -572,12 +1262,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="64351616"/>
+        <c:crossAx val="65373696"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="64351616"/>
+        <c:axId val="65373696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -588,7 +1278,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="64350080"/>
+        <c:crossAx val="65372160"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -695,11 +1385,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="65163264"/>
-        <c:axId val="65164800"/>
+        <c:axId val="65447808"/>
+        <c:axId val="65449344"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="65163264"/>
+        <c:axId val="65447808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -719,12 +1409,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="65164800"/>
+        <c:crossAx val="65449344"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="65164800"/>
+        <c:axId val="65449344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -735,7 +1425,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="65163264"/>
+        <c:crossAx val="65447808"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -842,11 +1532,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="65205760"/>
-        <c:axId val="65207296"/>
+        <c:axId val="65293696"/>
+        <c:axId val="65303680"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="65205760"/>
+        <c:axId val="65293696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -866,12 +1556,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="65207296"/>
+        <c:crossAx val="65303680"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="65207296"/>
+        <c:axId val="65303680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -882,7 +1572,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="65205760"/>
+        <c:crossAx val="65293696"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -933,7 +1623,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1078,11 +1767,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="87104128"/>
-        <c:axId val="75973760"/>
+        <c:axId val="74168192"/>
+        <c:axId val="74169728"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="87104128"/>
+        <c:axId val="74168192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1102,12 +1791,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="75973760"/>
+        <c:crossAx val="74169728"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="75973760"/>
+        <c:axId val="74169728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1118,14 +1807,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="87104128"/>
+        <c:crossAx val="74168192"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1170,7 +1858,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1251,11 +1938,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="87153280"/>
-        <c:axId val="76004352"/>
+        <c:axId val="61736832"/>
+        <c:axId val="61738368"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="87153280"/>
+        <c:axId val="61736832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1275,12 +1962,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="76004352"/>
+        <c:crossAx val="61738368"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="76004352"/>
+        <c:axId val="61738368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1291,14 +1978,590 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="87153280"/>
+        <c:crossAx val="61736832"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-CA"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Lateral Resolution (Axial)</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
       <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Proximal (B1)</c:v>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Lateral Resolution'!$A$3</c:f>
+              <c:numCache>
+                <c:formatCode>d\-mmm\-yy</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>42216</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Lateral Resolution'!$D$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>2.61</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Proximal (F1)</c:v>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Lateral Resolution'!$A$3</c:f>
+              <c:numCache>
+                <c:formatCode>d\-mmm\-yy</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>42216</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Lateral Resolution'!$D$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>3.23</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>Distal (B5)</c:v>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Lateral Resolution'!$A$3</c:f>
+              <c:numCache>
+                <c:formatCode>d\-mmm\-yy</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>42216</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Lateral Resolution'!$D$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>5.42</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>Distal (F5)</c:v>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Lateral Resolution'!$A$3</c:f>
+              <c:numCache>
+                <c:formatCode>d\-mmm\-yy</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>42216</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Lateral Resolution'!$D$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>5.47</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="74602752"/>
+        <c:axId val="74612736"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="74602752"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="d\-mmm\-yy" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr rot="-2100000" vert="horz"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="74612736"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="74612736"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="74602752"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-CA"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Lateral Resolution (Longitudinal)</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Filament 1</c:v>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Lateral Resolution'!$A$3</c:f>
+              <c:numCache>
+                <c:formatCode>d\-mmm\-yy</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>42216</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Lateral Resolution'!$K$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>2.74</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Filament 6</c:v>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Lateral Resolution'!$A$3</c:f>
+              <c:numCache>
+                <c:formatCode>d\-mmm\-yy</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>42216</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Lateral Resolution'!$K$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>2.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="75563776"/>
+        <c:axId val="75565312"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="75563776"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="d\-mmm\-yy" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr rot="-2100000" vert="horz"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="75565312"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="75565312"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="75563776"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-CA"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Axial Distance</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>B1 - B5</c:v>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Axial Distance'!$A$2</c:f>
+              <c:numCache>
+                <c:formatCode>d\-mmm\-yy</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>42216</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Axial Distance'!$D$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>39.96</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>F1 - F5</c:v>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Axial Distance'!$A$2</c:f>
+              <c:numCache>
+                <c:formatCode>d\-mmm\-yy</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>42216</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Axial Distance'!$D$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>39.81</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="75623808"/>
+        <c:axId val="75056256"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="75623808"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="d\-mmm\-yy" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr rot="-2100000" vert="horz"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="75056256"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="75056256"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="75623808"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1505,6 +2768,206 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>127000</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>269875</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>127000</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>393700</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>127000</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>355600</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>127000</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>117475</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>127000</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>384175</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing8.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>127000</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>527050</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1862,7 +3325,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="E2" sqref="E2"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1888,7 +3351,7 @@
         <v>5</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -1902,10 +3365,10 @@
         <v>11.06</v>
       </c>
       <c r="D2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -1921,11 +3384,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I6"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="E3" sqref="E3"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1946,12 +3409,14 @@
         <v>2</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C1" s="6"/>
       <c r="D1" s="6"/>
       <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
+      <c r="F1" s="6" t="s">
+        <v>10</v>
+      </c>
       <c r="G1" s="6"/>
       <c r="H1" s="6"/>
       <c r="I1" s="6"/>
@@ -1967,7 +3432,7 @@
         <v>5</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>3</v>
@@ -1979,7 +3444,7 @@
         <v>5</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -1993,10 +3458,10 @@
         <v>85.42</v>
       </c>
       <c r="D3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="5" t="s">
         <v>8</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>10</v>
       </c>
       <c r="F3">
         <v>78.8</v>
@@ -2005,24 +3470,16 @@
         <v>79.2</v>
       </c>
       <c r="H3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I3" s="5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="4"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="4"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="4"/>
+        <v>8</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="B1:I1"/>
+  <mergeCells count="2">
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="F1:I1"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="E3" r:id="rId1"/>
@@ -2039,10 +3496,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozenSplit"/>
-      <selection activeCell="D1" sqref="D1"/>
-      <selection pane="bottomLeft" sqref="A1:O6"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2064,10 +3520,10 @@
   <sheetData>
     <row r="1" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C1" s="6"/>
       <c r="D1" s="6"/>
@@ -2076,7 +3532,7 @@
       <c r="G1" s="6"/>
       <c r="H1" s="6"/>
       <c r="I1" s="6" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="J1" s="6"/>
       <c r="K1" s="6"/>
@@ -2092,16 +3548,16 @@
         <v>4</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>5</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="J2" s="2" t="s">
         <v>3</v>
@@ -2110,16 +3566,16 @@
         <v>4</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="N2" s="2" t="s">
         <v>5</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
@@ -2142,10 +3598,10 @@
         <v>11.97</v>
       </c>
       <c r="G3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="I3" s="2" t="s">
         <v>19</v>
@@ -2163,10 +3619,10 @@
         <v>13.36</v>
       </c>
       <c r="N3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="O3" s="5" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
@@ -2186,7 +3642,7 @@
         <v>3.65</v>
       </c>
       <c r="G4" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I4" s="2" t="s">
         <v>20</v>
@@ -2204,7 +3660,7 @@
         <v>9.67</v>
       </c>
       <c r="N4" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
@@ -2224,7 +3680,7 @@
         <v>17.239999999999998</v>
       </c>
       <c r="G5" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
@@ -2244,7 +3700,7 @@
         <v>21.39</v>
       </c>
       <c r="G6" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -2261,4 +3717,576 @@
   <drawing r:id="rId3"/>
   <legacyDrawing r:id="rId4"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:O6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" s="6"/>
+      <c r="K1" s="6"/>
+      <c r="L1" s="6"/>
+      <c r="M1" s="6"/>
+      <c r="N1" s="6"/>
+    </row>
+    <row r="2" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" s="4">
+        <v>42216</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3">
+        <v>1.27</v>
+      </c>
+      <c r="D3">
+        <v>2.61</v>
+      </c>
+      <c r="E3">
+        <v>1.34</v>
+      </c>
+      <c r="F3">
+        <v>69.03</v>
+      </c>
+      <c r="G3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J3">
+        <v>1.1100000000000001</v>
+      </c>
+      <c r="K3">
+        <v>2.74</v>
+      </c>
+      <c r="L3">
+        <v>1.63</v>
+      </c>
+      <c r="M3">
+        <v>84.54</v>
+      </c>
+      <c r="N3" t="s">
+        <v>11</v>
+      </c>
+      <c r="O3" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4">
+        <v>1.37</v>
+      </c>
+      <c r="D4">
+        <v>3.23</v>
+      </c>
+      <c r="E4">
+        <v>1.86</v>
+      </c>
+      <c r="F4">
+        <v>80.97</v>
+      </c>
+      <c r="G4" t="s">
+        <v>11</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J4">
+        <v>1</v>
+      </c>
+      <c r="K4">
+        <v>2.5</v>
+      </c>
+      <c r="L4">
+        <v>1.5</v>
+      </c>
+      <c r="M4">
+        <v>85.85</v>
+      </c>
+      <c r="N4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B5" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5">
+        <v>3.43</v>
+      </c>
+      <c r="D5">
+        <v>5.42</v>
+      </c>
+      <c r="E5">
+        <v>1.99</v>
+      </c>
+      <c r="F5">
+        <v>45.03</v>
+      </c>
+      <c r="G5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B6" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6">
+        <v>4.3</v>
+      </c>
+      <c r="D6">
+        <v>5.47</v>
+      </c>
+      <c r="E6">
+        <v>1.17</v>
+      </c>
+      <c r="F6">
+        <v>23.91</v>
+      </c>
+      <c r="G6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B1:H1"/>
+    <mergeCell ref="I1:N1"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="H3" r:id="rId1"/>
+    <hyperlink ref="O3" r:id="rId2"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <drawing r:id="rId3"/>
+  <legacyDrawing r:id="rId4"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="4">
+        <v>42216</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2">
+        <v>40</v>
+      </c>
+      <c r="D2">
+        <v>39.96</v>
+      </c>
+      <c r="E2">
+        <v>0.04</v>
+      </c>
+      <c r="F2">
+        <v>0.09</v>
+      </c>
+      <c r="G2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B3" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3">
+        <v>40</v>
+      </c>
+      <c r="D3">
+        <v>39.81</v>
+      </c>
+      <c r="E3">
+        <v>0.19</v>
+      </c>
+      <c r="F3">
+        <v>0.47</v>
+      </c>
+      <c r="G3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="H2" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:O4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" s="6"/>
+      <c r="K1" s="6"/>
+      <c r="L1" s="6"/>
+      <c r="M1" s="6"/>
+      <c r="N1" s="6"/>
+    </row>
+    <row r="2" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" s="4">
+        <v>42216</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3">
+        <v>40</v>
+      </c>
+      <c r="D3">
+        <v>40.86</v>
+      </c>
+      <c r="E3">
+        <v>0.86</v>
+      </c>
+      <c r="F3">
+        <v>2.13</v>
+      </c>
+      <c r="G3" t="s">
+        <v>7</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="J3">
+        <v>40</v>
+      </c>
+      <c r="K3">
+        <v>39.58</v>
+      </c>
+      <c r="L3">
+        <v>0.42</v>
+      </c>
+      <c r="M3">
+        <v>1.05</v>
+      </c>
+      <c r="N3" t="s">
+        <v>7</v>
+      </c>
+      <c r="O3" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B4" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4">
+        <v>40</v>
+      </c>
+      <c r="D4">
+        <v>40.97</v>
+      </c>
+      <c r="E4">
+        <v>0.97</v>
+      </c>
+      <c r="F4">
+        <v>2.38</v>
+      </c>
+      <c r="G4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B1:H1"/>
+    <mergeCell ref="I1:N1"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="H3" r:id="rId1"/>
+    <hyperlink ref="O3" r:id="rId2"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <drawing r:id="rId3"/>
+  <legacyDrawing r:id="rId4"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="8.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="4">
+        <v>42216</v>
+      </c>
+      <c r="B2">
+        <v>7</v>
+      </c>
+      <c r="C2">
+        <v>7.23</v>
+      </c>
+      <c r="D2">
+        <v>0.23</v>
+      </c>
+      <c r="E2">
+        <v>3.29</v>
+      </c>
+      <c r="F2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="G2" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Save exported images to folder with current date as name.
- Also improved sheet creation code, if not all test have been run yet.
</commit_message>
<xml_diff>
--- a/Log/ProstateBrachyQA Log.xlsx
+++ b/Log/ProstateBrachyQA Log.xlsx
@@ -378,7 +378,7 @@
     <t>Image</t>
   </si>
   <si>
-    <t>PASS</t>
+    <t>FAIL</t>
   </si>
   <si>
     <t>View Image</t>
@@ -390,7 +390,7 @@
     <t>Longitudinal Plane</t>
   </si>
   <si>
-    <t>FAIL</t>
+    <t>PASS</t>
   </si>
   <si>
     <t>Axial Resolution</t>
@@ -628,11 +628,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="63386752"/>
-        <c:axId val="63388288"/>
+        <c:axId val="62207104"/>
+        <c:axId val="62208640"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="63386752"/>
+        <c:axId val="62207104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -652,12 +652,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="63388288"/>
+        <c:crossAx val="62208640"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="63388288"/>
+        <c:axId val="62208640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -668,7 +668,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="63386752"/>
+        <c:crossAx val="62207104"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -800,11 +800,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="76581120"/>
-        <c:axId val="76587008"/>
+        <c:axId val="75872128"/>
+        <c:axId val="75873664"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="76581120"/>
+        <c:axId val="75872128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -824,12 +824,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="76587008"/>
+        <c:crossAx val="75873664"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="76587008"/>
+        <c:axId val="75873664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -840,7 +840,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="76581120"/>
+        <c:crossAx val="75872128"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -941,11 +941,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="76607488"/>
-        <c:axId val="76609024"/>
+        <c:axId val="75885952"/>
+        <c:axId val="75564160"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="76607488"/>
+        <c:axId val="75885952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -965,12 +965,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="76609024"/>
+        <c:crossAx val="75564160"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="76609024"/>
+        <c:axId val="75564160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -981,7 +981,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="76607488"/>
+        <c:crossAx val="75885952"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1090,11 +1090,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="91556864"/>
-        <c:axId val="89803008"/>
+        <c:axId val="82705024"/>
+        <c:axId val="81938304"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="91556864"/>
+        <c:axId val="82705024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1114,12 +1114,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="89803008"/>
+        <c:crossAx val="81938304"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="89803008"/>
+        <c:axId val="81938304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1130,7 +1130,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="91556864"/>
+        <c:crossAx val="82705024"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1223,7 +1223,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>11.06</c:v>
+                  <c:v>14.75</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1238,11 +1238,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="65372160"/>
-        <c:axId val="65373696"/>
+        <c:axId val="65088896"/>
+        <c:axId val="65111168"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="65372160"/>
+        <c:axId val="65088896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1262,12 +1262,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="65373696"/>
+        <c:crossAx val="65111168"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="65373696"/>
+        <c:axId val="65111168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1278,7 +1278,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="65372160"/>
+        <c:crossAx val="65088896"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1370,7 +1370,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>85.42</c:v>
+                  <c:v>80.180000000000007</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1385,11 +1385,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="65447808"/>
-        <c:axId val="65449344"/>
+        <c:axId val="65185280"/>
+        <c:axId val="65186816"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="65447808"/>
+        <c:axId val="65185280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1409,12 +1409,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="65449344"/>
+        <c:crossAx val="65186816"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="65449344"/>
+        <c:axId val="65186816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1425,7 +1425,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="65447808"/>
+        <c:crossAx val="65185280"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1517,7 +1517,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>79.2</c:v>
+                  <c:v>63.94</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1532,11 +1532,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="65293696"/>
-        <c:axId val="65303680"/>
+        <c:axId val="48708608"/>
+        <c:axId val="48718592"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="65293696"/>
+        <c:axId val="48708608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1556,12 +1556,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="65303680"/>
+        <c:crossAx val="48718592"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="65303680"/>
+        <c:axId val="48718592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1572,7 +1572,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="65293696"/>
+        <c:crossAx val="48708608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1767,11 +1767,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="74168192"/>
-        <c:axId val="74169728"/>
+        <c:axId val="66831488"/>
+        <c:axId val="66833024"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="74168192"/>
+        <c:axId val="66831488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1791,12 +1791,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="74169728"/>
+        <c:crossAx val="66833024"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="74169728"/>
+        <c:axId val="66833024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1807,7 +1807,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="74168192"/>
+        <c:crossAx val="66831488"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1938,11 +1938,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="61736832"/>
-        <c:axId val="61738368"/>
+        <c:axId val="66852736"/>
+        <c:axId val="66854272"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="61736832"/>
+        <c:axId val="66852736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1962,12 +1962,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="61738368"/>
+        <c:crossAx val="66854272"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="61738368"/>
+        <c:axId val="66854272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1978,7 +1978,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="61736832"/>
+        <c:crossAx val="66852736"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2173,11 +2173,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="74602752"/>
-        <c:axId val="74612736"/>
+        <c:axId val="74537216"/>
+        <c:axId val="74547200"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="74602752"/>
+        <c:axId val="74537216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2197,12 +2197,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="74612736"/>
+        <c:crossAx val="74547200"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="74612736"/>
+        <c:axId val="74547200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2213,7 +2213,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="74602752"/>
+        <c:crossAx val="74537216"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2344,11 +2344,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="75563776"/>
-        <c:axId val="75565312"/>
+        <c:axId val="65474944"/>
+        <c:axId val="65476480"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="75563776"/>
+        <c:axId val="65474944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2368,12 +2368,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="75565312"/>
+        <c:crossAx val="65476480"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="75565312"/>
+        <c:axId val="65476480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2384,7 +2384,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="75563776"/>
+        <c:crossAx val="65474944"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2515,11 +2515,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="75623808"/>
-        <c:axId val="75056256"/>
+        <c:axId val="65526784"/>
+        <c:axId val="75510528"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="75623808"/>
+        <c:axId val="65526784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2539,12 +2539,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="75056256"/>
+        <c:crossAx val="75510528"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="75056256"/>
+        <c:axId val="75510528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2555,7 +2555,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="75623808"/>
+        <c:crossAx val="65526784"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3362,7 +3362,7 @@
         <v>10.7</v>
       </c>
       <c r="C2">
-        <v>11.06</v>
+        <v>14.75</v>
       </c>
       <c r="D2" t="s">
         <v>7</v>
@@ -3455,7 +3455,7 @@
         <v>75.3</v>
       </c>
       <c r="C3">
-        <v>85.42</v>
+        <v>80.180000000000007</v>
       </c>
       <c r="D3" t="s">
         <v>11</v>
@@ -3467,7 +3467,7 @@
         <v>78.8</v>
       </c>
       <c r="G3">
-        <v>79.2</v>
+        <v>63.94</v>
       </c>
       <c r="H3" t="s">
         <v>7</v>
@@ -3598,7 +3598,7 @@
         <v>11.97</v>
       </c>
       <c r="G3" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="H3" s="5" t="s">
         <v>8</v>
@@ -3619,7 +3619,7 @@
         <v>13.36</v>
       </c>
       <c r="N3" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="O3" s="5" t="s">
         <v>8</v>
@@ -3642,7 +3642,7 @@
         <v>3.65</v>
       </c>
       <c r="G4" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="I4" s="2" t="s">
         <v>20</v>
@@ -3660,7 +3660,7 @@
         <v>9.67</v>
       </c>
       <c r="N4" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
@@ -3680,7 +3680,7 @@
         <v>17.239999999999998</v>
       </c>
       <c r="G5" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
@@ -3700,7 +3700,7 @@
         <v>21.39</v>
       </c>
       <c r="G6" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -3825,7 +3825,7 @@
         <v>69.03</v>
       </c>
       <c r="G3" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="H3" s="5" t="s">
         <v>8</v>
@@ -3846,7 +3846,7 @@
         <v>84.54</v>
       </c>
       <c r="N3" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="O3" s="5" t="s">
         <v>8</v>
@@ -3869,7 +3869,7 @@
         <v>80.97</v>
       </c>
       <c r="G4" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="I4" s="2" t="s">
         <v>20</v>
@@ -3887,7 +3887,7 @@
         <v>85.85</v>
       </c>
       <c r="N4" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
@@ -3907,7 +3907,7 @@
         <v>45.03</v>
       </c>
       <c r="G5" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
@@ -3927,7 +3927,7 @@
         <v>23.91</v>
       </c>
       <c r="G6" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -4009,7 +4009,7 @@
         <v>0.09</v>
       </c>
       <c r="G2" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="H2" s="5" t="s">
         <v>8</v>
@@ -4032,7 +4032,7 @@
         <v>0.47</v>
       </c>
       <c r="G3" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -4152,7 +4152,7 @@
         <v>2.13</v>
       </c>
       <c r="G3" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="H3" s="5" t="s">
         <v>8</v>
@@ -4173,7 +4173,7 @@
         <v>1.05</v>
       </c>
       <c r="N3" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="O3" s="5" t="s">
         <v>8</v>
@@ -4196,7 +4196,7 @@
         <v>2.38</v>
       </c>
       <c r="G4" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -4274,7 +4274,7 @@
         <v>3.29</v>
       </c>
       <c r="F2" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="G2" s="5" t="s">
         <v>8</v>

</xml_diff>